<commit_message>
ENH: Checkboxes to select plotted variables
</commit_message>
<xml_diff>
--- a/inst/examples/DRT/model.xlsx
+++ b/inst/examples/DRT/model.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="87">
   <si>
     <t>name</t>
   </si>
@@ -30,61 +30,61 @@
     <t>description</t>
   </si>
   <si>
+    <t>default</t>
+  </si>
+  <si>
+    <t>lower</t>
+  </si>
+  <si>
+    <t>upper</t>
+  </si>
+  <si>
+    <t>label</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>mg/L</t>
+  </si>
+  <si>
+    <t>concentration of antibiotic</t>
+  </si>
+  <si>
+    <t>Antibiotic</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>cells/ml</t>
+  </si>
+  <si>
+    <t>abundance of donor</t>
+  </si>
+  <si>
+    <t>Donors</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>abundance of recipient</t>
+  </si>
+  <si>
+    <t>Recipients</t>
+  </si>
+  <si>
+    <t>T</t>
+  </si>
+  <si>
+    <t>abundance of transconjugant</t>
+  </si>
+  <si>
+    <t>Transconj.</t>
+  </si>
+  <si>
     <t>user</t>
-  </si>
-  <si>
-    <t>default</t>
-  </si>
-  <si>
-    <t>lower</t>
-  </si>
-  <si>
-    <t>upper</t>
-  </si>
-  <si>
-    <t>label</t>
-  </si>
-  <si>
-    <t>A</t>
-  </si>
-  <si>
-    <t>mg/L</t>
-  </si>
-  <si>
-    <t>concentration of antibiotic</t>
-  </si>
-  <si>
-    <t>Antibiotic</t>
-  </si>
-  <si>
-    <t>D</t>
-  </si>
-  <si>
-    <t>cells/ml</t>
-  </si>
-  <si>
-    <t>abundance of donor</t>
-  </si>
-  <si>
-    <t>Donors</t>
-  </si>
-  <si>
-    <t>R</t>
-  </si>
-  <si>
-    <t>abundance of recipient</t>
-  </si>
-  <si>
-    <t>Recipients</t>
-  </si>
-  <si>
-    <t>T</t>
-  </si>
-  <si>
-    <t>abundance of transconjugant</t>
-  </si>
-  <si>
-    <t>Transconj.</t>
   </si>
   <si>
     <t>K</t>
@@ -286,17 +286,17 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="GENERAL"/>
-    <numFmt numFmtId="165" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
-    <numFmt numFmtId="166" formatCode="0.00E+000"/>
-    <numFmt numFmtId="167" formatCode="@"/>
+    <numFmt numFmtId="165" formatCode="0.00E+000"/>
+    <numFmt numFmtId="166" formatCode="@"/>
   </numFmts>
   <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -318,6 +318,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="4">
@@ -387,19 +388,19 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="166" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -480,10 +481,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J10" activeCellId="0" sqref="J10"/>
+      <selection pane="topLeft" activeCell="E12" activeCellId="0" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -515,99 +516,87 @@
       <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="C2" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2" s="2" t="b">
-        <v>1</v>
+      <c r="D2" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="E2" s="0" t="n">
         <v>0</v>
       </c>
       <c r="F2" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="G2" s="0" t="n">
         <v>2.5</v>
       </c>
-      <c r="H2" s="0" t="s">
-        <v>11</v>
+      <c r="G2" s="0" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="C3" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="D3" s="2" t="n">
+        <v>100000</v>
+      </c>
+      <c r="E3" s="2" t="n">
+        <v>100000</v>
+      </c>
+      <c r="F3" s="2" t="n">
+        <v>100000</v>
+      </c>
+      <c r="G3" s="0" t="s">
         <v>14</v>
-      </c>
-      <c r="D3" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E3" s="3" t="n">
-        <v>100000</v>
-      </c>
-      <c r="F3" s="3" t="n">
-        <v>100000</v>
-      </c>
-      <c r="G3" s="3" t="n">
-        <v>100000</v>
-      </c>
-      <c r="H3" s="0" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" s="0" t="s">
+      <c r="D4" s="2" t="n">
+        <v>100000</v>
+      </c>
+      <c r="E4" s="2" t="n">
+        <v>100000</v>
+      </c>
+      <c r="F4" s="2" t="n">
+        <v>100000</v>
+      </c>
+      <c r="G4" s="0" t="s">
         <v>17</v>
-      </c>
-      <c r="D4" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E4" s="3" t="n">
-        <v>100000</v>
-      </c>
-      <c r="F4" s="3" t="n">
-        <v>100000</v>
-      </c>
-      <c r="G4" s="3" t="n">
-        <v>100000</v>
-      </c>
-      <c r="H4" s="0" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="B5" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="D5" s="2" t="b">
+      <c r="D5" s="0" t="n">
         <v>1</v>
       </c>
       <c r="E5" s="0" t="n">
@@ -616,11 +605,8 @@
       <c r="F5" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="G5" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="H5" s="0" t="s">
-        <v>21</v>
+      <c r="G5" s="0" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -642,7 +628,7 @@
   <dimension ref="A1:H19"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I9" activeCellId="0" sqref="I9"/>
+      <selection pane="topLeft" activeCell="D25" activeCellId="0" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -655,29 +641,29 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="F1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="G1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="H1" s="3" t="s">
         <v>6</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -685,21 +671,22 @@
         <v>22</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C2" s="0" t="s">
         <v>23</v>
       </c>
-      <c r="D2" s="2" t="b">
+      <c r="D2" s="4" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="E2" s="3" t="n">
+      <c r="E2" s="2" t="n">
         <v>3430000000</v>
       </c>
-      <c r="F2" s="3" t="n">
+      <c r="F2" s="2" t="n">
         <v>1720000000</v>
       </c>
-      <c r="G2" s="3" t="n">
+      <c r="G2" s="2" t="n">
         <v>6860000000</v>
       </c>
       <c r="H2" s="0" t="s">
@@ -716,16 +703,19 @@
       <c r="C3" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="D3" s="2" t="b">
-        <v>1</v>
+      <c r="D3" s="4" t="inlineStr">
+        <f aca="false">TRUE()</f>
+        <is>
+          <t/>
+        </is>
       </c>
       <c r="E3" s="0" t="n">
         <v>0.1</v>
       </c>
-      <c r="F3" s="3" t="n">
+      <c r="F3" s="2" t="n">
         <v>0.05</v>
       </c>
-      <c r="G3" s="3" t="n">
+      <c r="G3" s="2" t="n">
         <v>0.2</v>
       </c>
       <c r="H3" s="0" t="s">
@@ -742,16 +732,19 @@
       <c r="C4" s="0" t="s">
         <v>30</v>
       </c>
-      <c r="D4" s="2" t="b">
-        <v>1</v>
+      <c r="D4" s="4" t="inlineStr">
+        <f aca="false">TRUE()</f>
+        <is>
+          <t/>
+        </is>
       </c>
       <c r="E4" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="F4" s="3" t="n">
+      <c r="F4" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G4" s="3" t="n">
+      <c r="G4" s="2" t="n">
         <v>0</v>
       </c>
       <c r="H4" s="0" t="s">
@@ -768,16 +761,19 @@
       <c r="C5" s="0" t="s">
         <v>33</v>
       </c>
-      <c r="D5" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E5" s="3" t="n">
+      <c r="D5" s="4" t="inlineStr">
+        <f aca="false">TRUE()</f>
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="E5" s="2" t="n">
         <v>5E-006</v>
       </c>
-      <c r="F5" s="3" t="n">
+      <c r="F5" s="2" t="n">
         <v>2.5E-006</v>
       </c>
-      <c r="G5" s="3" t="n">
+      <c r="G5" s="2" t="n">
         <v>1E-005</v>
       </c>
       <c r="H5" s="0" t="s">
@@ -794,16 +790,19 @@
       <c r="C6" s="0" t="s">
         <v>37</v>
       </c>
-      <c r="D6" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E6" s="3" t="n">
+      <c r="D6" s="4" t="inlineStr">
+        <f aca="false">TRUE()</f>
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="E6" s="2" t="n">
         <v>1.1E-011</v>
       </c>
-      <c r="F6" s="3" t="n">
+      <c r="F6" s="2" t="n">
         <v>5.5E-012</v>
       </c>
-      <c r="G6" s="3" t="n">
+      <c r="G6" s="2" t="n">
         <v>2.2E-011</v>
       </c>
       <c r="H6" s="0" t="s">
@@ -820,16 +819,19 @@
       <c r="C7" s="0" t="s">
         <v>40</v>
       </c>
-      <c r="D7" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E7" s="3" t="n">
+      <c r="D7" s="4" t="inlineStr">
+        <f aca="false">TRUE()</f>
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="E7" s="2" t="n">
         <v>1.1E-011</v>
       </c>
-      <c r="F7" s="3" t="n">
+      <c r="F7" s="2" t="n">
         <v>5.5E-012</v>
       </c>
-      <c r="G7" s="3" t="n">
+      <c r="G7" s="2" t="n">
         <v>2.2E-011</v>
       </c>
       <c r="H7" s="0" t="s">
@@ -846,7 +848,8 @@
       <c r="C8" s="0" t="s">
         <v>44</v>
       </c>
-      <c r="D8" s="2" t="b">
+      <c r="D8" s="4" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="E8" s="0" t="n">
@@ -872,8 +875,11 @@
       <c r="C9" s="0" t="s">
         <v>44</v>
       </c>
-      <c r="D9" s="2" t="b">
-        <v>0</v>
+      <c r="D9" s="4" t="inlineStr">
+        <f aca="false">FALSE()</f>
+        <is>
+          <t/>
+        </is>
       </c>
       <c r="E9" s="0" t="n">
         <v>0.1</v>
@@ -898,8 +904,11 @@
       <c r="C10" s="0" t="s">
         <v>44</v>
       </c>
-      <c r="D10" s="2" t="b">
-        <v>0</v>
+      <c r="D10" s="4" t="inlineStr">
+        <f aca="false">FALSE()</f>
+        <is>
+          <t/>
+        </is>
       </c>
       <c r="E10" s="0" t="n">
         <v>23.42</v>
@@ -924,8 +933,11 @@
       <c r="C11" s="0" t="s">
         <v>44</v>
       </c>
-      <c r="D11" s="2" t="b">
-        <v>0</v>
+      <c r="D11" s="4" t="inlineStr">
+        <f aca="false">FALSE()</f>
+        <is>
+          <t/>
+        </is>
       </c>
       <c r="E11" s="0" t="n">
         <v>4.52</v>
@@ -950,8 +962,11 @@
       <c r="C12" s="0" t="s">
         <v>44</v>
       </c>
-      <c r="D12" s="2" t="b">
-        <v>0</v>
+      <c r="D12" s="4" t="inlineStr">
+        <f aca="false">FALSE()</f>
+        <is>
+          <t/>
+        </is>
       </c>
       <c r="E12" s="0" t="n">
         <v>0.22</v>
@@ -976,8 +991,11 @@
       <c r="C13" s="0" t="s">
         <v>44</v>
       </c>
-      <c r="D13" s="2" t="b">
-        <v>0</v>
+      <c r="D13" s="4" t="inlineStr">
+        <f aca="false">FALSE()</f>
+        <is>
+          <t/>
+        </is>
       </c>
       <c r="E13" s="0" t="n">
         <v>0.14</v>
@@ -1002,8 +1020,11 @@
       <c r="C14" s="0" t="s">
         <v>44</v>
       </c>
-      <c r="D14" s="2" t="b">
-        <v>0</v>
+      <c r="D14" s="4" t="inlineStr">
+        <f aca="false">FALSE()</f>
+        <is>
+          <t/>
+        </is>
       </c>
       <c r="E14" s="0" t="n">
         <v>29.6</v>
@@ -1028,8 +1049,11 @@
       <c r="C15" s="0" t="s">
         <v>44</v>
       </c>
-      <c r="D15" s="2" t="b">
-        <v>0</v>
+      <c r="D15" s="4" t="inlineStr">
+        <f aca="false">FALSE()</f>
+        <is>
+          <t/>
+        </is>
       </c>
       <c r="E15" s="0" t="n">
         <v>0.73</v>
@@ -1054,8 +1078,11 @@
       <c r="C16" s="0" t="s">
         <v>44</v>
       </c>
-      <c r="D16" s="2" t="b">
-        <v>0</v>
+      <c r="D16" s="4" t="inlineStr">
+        <f aca="false">FALSE()</f>
+        <is>
+          <t/>
+        </is>
       </c>
       <c r="E16" s="0" t="n">
         <v>0.24</v>
@@ -1080,8 +1107,11 @@
       <c r="C17" s="0" t="s">
         <v>44</v>
       </c>
-      <c r="D17" s="2" t="b">
-        <v>0</v>
+      <c r="D17" s="4" t="inlineStr">
+        <f aca="false">FALSE()</f>
+        <is>
+          <t/>
+        </is>
       </c>
       <c r="E17" s="0" t="n">
         <v>0.08</v>
@@ -1106,8 +1136,11 @@
       <c r="C18" s="0" t="s">
         <v>44</v>
       </c>
-      <c r="D18" s="2" t="b">
-        <v>0</v>
+      <c r="D18" s="4" t="inlineStr">
+        <f aca="false">FALSE()</f>
+        <is>
+          <t/>
+        </is>
       </c>
       <c r="E18" s="0" t="n">
         <v>25.19</v>
@@ -1132,8 +1165,11 @@
       <c r="C19" s="0" t="s">
         <v>44</v>
       </c>
-      <c r="D19" s="2" t="b">
-        <v>0</v>
+      <c r="D19" s="4" t="inlineStr">
+        <f aca="false">FALSE()</f>
+        <is>
+          <t/>
+        </is>
       </c>
       <c r="E19" s="0" t="n">
         <v>4.15</v>
@@ -1151,7 +1187,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -1179,13 +1215,13 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
     </row>
@@ -1199,7 +1235,7 @@
       <c r="C2" s="0" t="s">
         <v>57</v>
       </c>
-      <c r="E2" s="2"/>
+      <c r="E2" s="4"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
@@ -1211,12 +1247,12 @@
       <c r="C3" s="0" t="s">
         <v>59</v>
       </c>
-      <c r="E3" s="2"/>
+      <c r="E3" s="4"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -1290,7 +1326,7 @@
         <v>66</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C4" s="0" t="s">
         <v>62</v>
@@ -1330,7 +1366,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -1352,7 +1388,7 @@
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="2" min="1" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="43.5867346938776"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="43.5867346938776"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
@@ -1363,146 +1399,146 @@
       <c r="B1" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="5" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B2" s="0" t="s">
         <v>70</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="6" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B3" s="0" t="s">
         <v>61</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="6" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B4" s="0" t="s">
         <v>64</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="6" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B5" s="0" t="s">
         <v>68</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="6" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B6" s="0" t="s">
         <v>61</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C6" s="6" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B7" s="0" t="s">
         <v>64</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="C7" s="6" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B8" s="0" t="s">
         <v>68</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="C8" s="6" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B9" s="0" t="s">
         <v>66</v>
       </c>
-      <c r="C9" s="5" t="s">
+      <c r="C9" s="6" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B10" s="0" t="s">
         <v>61</v>
       </c>
-      <c r="C10" s="5" t="s">
+      <c r="C10" s="6" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B11" s="0" t="s">
         <v>64</v>
       </c>
-      <c r="C11" s="5" t="s">
+      <c r="C11" s="6" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B12" s="0" t="s">
         <v>68</v>
       </c>
-      <c r="C12" s="5" t="s">
+      <c r="C12" s="6" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B13" s="0" t="s">
         <v>66</v>
       </c>
-      <c r="C13" s="5" t="s">
+      <c r="C13" s="6" t="s">
         <v>86</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>

<commit_message>
MIN: Script to test GUI locally (not using installed package)
</commit_message>
<xml_diff>
--- a/inst/examples/DRT/model.xlsx
+++ b/inst/examples/DRT/model.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="196" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="196" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="vars" sheetId="1" state="visible" r:id="rId2"/>
@@ -375,7 +375,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -389,10 +389,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -483,7 +479,7 @@
   </sheetPr>
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E12" activeCellId="0" sqref="E12"/>
     </sheetView>
   </sheetViews>
@@ -627,8 +623,8 @@
   </sheetPr>
   <dimension ref="A1:H19"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D25" activeCellId="0" sqref="D25"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D20" activeCellId="0" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -676,8 +672,7 @@
       <c r="C2" s="0" t="s">
         <v>23</v>
       </c>
-      <c r="D2" s="4" t="n">
-        <f aca="false">TRUE()</f>
+      <c r="D2" s="0" t="n">
         <v>1</v>
       </c>
       <c r="E2" s="2" t="n">
@@ -703,11 +698,8 @@
       <c r="C3" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="D3" s="4" t="inlineStr">
-        <f aca="false">TRUE()</f>
-        <is>
-          <t/>
-        </is>
+      <c r="D3" s="0" t="n">
+        <v>1</v>
       </c>
       <c r="E3" s="0" t="n">
         <v>0.1</v>
@@ -732,11 +724,8 @@
       <c r="C4" s="0" t="s">
         <v>30</v>
       </c>
-      <c r="D4" s="4" t="inlineStr">
-        <f aca="false">TRUE()</f>
-        <is>
-          <t/>
-        </is>
+      <c r="D4" s="0" t="n">
+        <v>1</v>
       </c>
       <c r="E4" s="0" t="n">
         <v>0</v>
@@ -761,11 +750,8 @@
       <c r="C5" s="0" t="s">
         <v>33</v>
       </c>
-      <c r="D5" s="4" t="inlineStr">
-        <f aca="false">TRUE()</f>
-        <is>
-          <t/>
-        </is>
+      <c r="D5" s="0" t="n">
+        <v>1</v>
       </c>
       <c r="E5" s="2" t="n">
         <v>5E-006</v>
@@ -790,11 +776,8 @@
       <c r="C6" s="0" t="s">
         <v>37</v>
       </c>
-      <c r="D6" s="4" t="inlineStr">
-        <f aca="false">TRUE()</f>
-        <is>
-          <t/>
-        </is>
+      <c r="D6" s="0" t="n">
+        <v>1</v>
       </c>
       <c r="E6" s="2" t="n">
         <v>1.1E-011</v>
@@ -819,11 +802,8 @@
       <c r="C7" s="0" t="s">
         <v>40</v>
       </c>
-      <c r="D7" s="4" t="inlineStr">
-        <f aca="false">TRUE()</f>
-        <is>
-          <t/>
-        </is>
+      <c r="D7" s="0" t="n">
+        <v>1</v>
       </c>
       <c r="E7" s="2" t="n">
         <v>1.1E-011</v>
@@ -848,8 +828,7 @@
       <c r="C8" s="0" t="s">
         <v>44</v>
       </c>
-      <c r="D8" s="4" t="n">
-        <f aca="false">FALSE()</f>
+      <c r="D8" s="0" t="n">
         <v>0</v>
       </c>
       <c r="E8" s="0" t="n">
@@ -875,11 +854,8 @@
       <c r="C9" s="0" t="s">
         <v>44</v>
       </c>
-      <c r="D9" s="4" t="inlineStr">
-        <f aca="false">FALSE()</f>
-        <is>
-          <t/>
-        </is>
+      <c r="D9" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="E9" s="0" t="n">
         <v>0.1</v>
@@ -904,11 +880,8 @@
       <c r="C10" s="0" t="s">
         <v>44</v>
       </c>
-      <c r="D10" s="4" t="inlineStr">
-        <f aca="false">FALSE()</f>
-        <is>
-          <t/>
-        </is>
+      <c r="D10" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="E10" s="0" t="n">
         <v>23.42</v>
@@ -933,11 +906,8 @@
       <c r="C11" s="0" t="s">
         <v>44</v>
       </c>
-      <c r="D11" s="4" t="inlineStr">
-        <f aca="false">FALSE()</f>
-        <is>
-          <t/>
-        </is>
+      <c r="D11" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="E11" s="0" t="n">
         <v>4.52</v>
@@ -962,11 +932,8 @@
       <c r="C12" s="0" t="s">
         <v>44</v>
       </c>
-      <c r="D12" s="4" t="inlineStr">
-        <f aca="false">FALSE()</f>
-        <is>
-          <t/>
-        </is>
+      <c r="D12" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="E12" s="0" t="n">
         <v>0.22</v>
@@ -991,11 +958,8 @@
       <c r="C13" s="0" t="s">
         <v>44</v>
       </c>
-      <c r="D13" s="4" t="inlineStr">
-        <f aca="false">FALSE()</f>
-        <is>
-          <t/>
-        </is>
+      <c r="D13" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="E13" s="0" t="n">
         <v>0.14</v>
@@ -1020,11 +984,8 @@
       <c r="C14" s="0" t="s">
         <v>44</v>
       </c>
-      <c r="D14" s="4" t="inlineStr">
-        <f aca="false">FALSE()</f>
-        <is>
-          <t/>
-        </is>
+      <c r="D14" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="E14" s="0" t="n">
         <v>29.6</v>
@@ -1049,11 +1010,8 @@
       <c r="C15" s="0" t="s">
         <v>44</v>
       </c>
-      <c r="D15" s="4" t="inlineStr">
-        <f aca="false">FALSE()</f>
-        <is>
-          <t/>
-        </is>
+      <c r="D15" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="E15" s="0" t="n">
         <v>0.73</v>
@@ -1078,11 +1036,8 @@
       <c r="C16" s="0" t="s">
         <v>44</v>
       </c>
-      <c r="D16" s="4" t="inlineStr">
-        <f aca="false">FALSE()</f>
-        <is>
-          <t/>
-        </is>
+      <c r="D16" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="E16" s="0" t="n">
         <v>0.24</v>
@@ -1107,11 +1062,8 @@
       <c r="C17" s="0" t="s">
         <v>44</v>
       </c>
-      <c r="D17" s="4" t="inlineStr">
-        <f aca="false">FALSE()</f>
-        <is>
-          <t/>
-        </is>
+      <c r="D17" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="E17" s="0" t="n">
         <v>0.08</v>
@@ -1136,11 +1088,8 @@
       <c r="C18" s="0" t="s">
         <v>44</v>
       </c>
-      <c r="D18" s="4" t="inlineStr">
-        <f aca="false">FALSE()</f>
-        <is>
-          <t/>
-        </is>
+      <c r="D18" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="E18" s="0" t="n">
         <v>25.19</v>
@@ -1165,11 +1114,8 @@
       <c r="C19" s="0" t="s">
         <v>44</v>
       </c>
-      <c r="D19" s="4" t="inlineStr">
-        <f aca="false">FALSE()</f>
-        <is>
-          <t/>
-        </is>
+      <c r="D19" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="E19" s="0" t="n">
         <v>4.15</v>
@@ -1200,7 +1146,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F9" activeCellId="0" sqref="F9"/>
@@ -1235,7 +1181,6 @@
       <c r="C2" s="0" t="s">
         <v>57</v>
       </c>
-      <c r="E2" s="4"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
@@ -1247,7 +1192,6 @@
       <c r="C3" s="0" t="s">
         <v>59</v>
       </c>
-      <c r="E3" s="4"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -1399,7 +1343,7 @@
       <c r="B1" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="4" t="s">
         <v>60</v>
       </c>
     </row>
@@ -1410,7 +1354,7 @@
       <c r="B2" s="0" t="s">
         <v>70</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="5" t="s">
         <v>75</v>
       </c>
     </row>
@@ -1421,7 +1365,7 @@
       <c r="B3" s="0" t="s">
         <v>61</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="5" t="s">
         <v>76</v>
       </c>
     </row>
@@ -1432,7 +1376,7 @@
       <c r="B4" s="0" t="s">
         <v>64</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="5" t="s">
         <v>77</v>
       </c>
     </row>
@@ -1443,7 +1387,7 @@
       <c r="B5" s="0" t="s">
         <v>68</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="5" t="s">
         <v>78</v>
       </c>
     </row>
@@ -1454,7 +1398,7 @@
       <c r="B6" s="0" t="s">
         <v>61</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="5" t="s">
         <v>79</v>
       </c>
     </row>
@@ -1465,7 +1409,7 @@
       <c r="B7" s="0" t="s">
         <v>64</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C7" s="5" t="s">
         <v>80</v>
       </c>
     </row>
@@ -1476,7 +1420,7 @@
       <c r="B8" s="0" t="s">
         <v>68</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="C8" s="5" t="s">
         <v>81</v>
       </c>
     </row>
@@ -1487,7 +1431,7 @@
       <c r="B9" s="0" t="s">
         <v>66</v>
       </c>
-      <c r="C9" s="6" t="s">
+      <c r="C9" s="5" t="s">
         <v>82</v>
       </c>
     </row>
@@ -1498,7 +1442,7 @@
       <c r="B10" s="0" t="s">
         <v>61</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="C10" s="5" t="s">
         <v>83</v>
       </c>
     </row>
@@ -1509,7 +1453,7 @@
       <c r="B11" s="0" t="s">
         <v>64</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="C11" s="5" t="s">
         <v>84</v>
       </c>
     </row>
@@ -1520,7 +1464,7 @@
       <c r="B12" s="0" t="s">
         <v>68</v>
       </c>
-      <c r="C12" s="6" t="s">
+      <c r="C12" s="5" t="s">
         <v>85</v>
       </c>
     </row>
@@ -1531,7 +1475,7 @@
       <c r="B13" s="0" t="s">
         <v>66</v>
       </c>
-      <c r="C13" s="6" t="s">
+      <c r="C13" s="5" t="s">
         <v>86</v>
       </c>
     </row>

</xml_diff>

<commit_message>
MIN: Added parameter in example model (allows for direct specification of growth rate)
</commit_message>
<xml_diff>
--- a/inst/examples/DRT/model.xlsx
+++ b/inst/examples/DRT/model.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="196" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="196" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="vars" sheetId="1" state="visible" r:id="rId2"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="88">
   <si>
     <t>name</t>
   </si>
@@ -189,6 +189,9 @@
     <t>qT</t>
   </si>
   <si>
+    <t>z</t>
+  </si>
+  <si>
     <t>fun</t>
   </si>
   <si>
@@ -249,34 +252,34 @@
     <t>-1</t>
   </si>
   <si>
-    <t>fun(A,aD,bD,pD,qD) * D</t>
+    <t>fun(A,z,aD,bD,pD,qD) * D</t>
   </si>
   <si>
     <t>-D</t>
   </si>
   <si>
-    <t>-fun(A,aD,bD,pD,qD) * D</t>
-  </si>
-  <si>
-    <t>fun(A,aR,bR,pR,qR) * R</t>
+    <t>-fun(A,z,aD,bD,pD,qD) * D</t>
+  </si>
+  <si>
+    <t>fun(A,z,aR,bR,pR,qR) * R</t>
   </si>
   <si>
     <t>-R</t>
   </si>
   <si>
-    <t>fun(A,aD,bD,pD,qD) * D + fun(A,aT,bT,pT,qT) * T</t>
+    <t>fun(A,z,aD,bD,pD,qD) * D + fun(A,z,aT,bT,pT,qT) * T</t>
   </si>
   <si>
     <t>-gammaDR * D - gammaTR * T</t>
   </si>
   <si>
-    <t>fun(A,aT,bT,pT,qT) * T</t>
+    <t>fun(A,z,aT,bT,pT,qT) * T</t>
   </si>
   <si>
     <t>-T</t>
   </si>
   <si>
-    <t>-fun(A,aT,bT,pT,qT) * T</t>
+    <t>-fun(A,z,aT,bT,pT,qT) * T</t>
   </si>
   <si>
     <t>gammaDR * D + gammaTR * T</t>
@@ -621,10 +624,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H19"/>
+  <dimension ref="A1:H20"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D20" activeCellId="0" sqref="D20"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H21" activeCellId="0" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1128,6 +1131,32 @@
       </c>
       <c r="H19" s="0" t="s">
         <v>55</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="B20" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="C20" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="D20" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E20" s="0" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="F20" s="0" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="G20" s="0" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="H20" s="0" t="s">
+        <v>56</v>
       </c>
     </row>
   </sheetData>
@@ -1173,24 +1202,24 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B2" s="0" t="s">
         <v>43</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B3" s="0" t="s">
         <v>43</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -1234,32 +1263,32 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B2" s="0" t="s">
         <v>43</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B3" s="0" t="s">
         <v>26</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D3" s="0" t="s">
         <v>25</v>
@@ -1267,44 +1296,44 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B4" s="0" t="s">
         <v>12</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B5" s="0" t="s">
         <v>26</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B6" s="0" t="s">
         <v>26</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
   </sheetData>
@@ -1325,8 +1354,8 @@
   </sheetPr>
   <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F13" activeCellId="0" sqref="F13"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C13" activeCellId="0" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1338,13 +1367,13 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1352,10 +1381,10 @@
         <v>7</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1363,10 +1392,10 @@
         <v>11</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1374,10 +1403,10 @@
         <v>11</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1385,10 +1414,10 @@
         <v>11</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1396,10 +1425,10 @@
         <v>15</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1407,10 +1436,10 @@
         <v>15</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1418,10 +1447,10 @@
         <v>15</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1429,10 +1458,10 @@
         <v>15</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1440,10 +1469,10 @@
         <v>18</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1451,10 +1480,10 @@
         <v>18</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1462,10 +1491,10 @@
         <v>18</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1473,10 +1502,10 @@
         <v>18</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ENH: Re-defined example model to facilitate parameter fitting
</commit_message>
<xml_diff>
--- a/inst/examples/DRT/model.xlsx
+++ b/inst/examples/DRT/model.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="196" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="196" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="vars" sheetId="1" state="visible" r:id="rId2"/>
@@ -90,69 +90,69 @@
     <t>K</t>
   </si>
   <si>
+    <t>Carrying c.</t>
+  </si>
+  <si>
     <t>carrying capacity (for any species)</t>
   </si>
   <si>
-    <t>Carrying c.</t>
-  </si>
-  <si>
     <t>g</t>
   </si>
   <si>
     <t>1/h</t>
   </si>
   <si>
+    <t>Loss const.</t>
+  </si>
+  <si>
     <t>loss constant</t>
   </si>
   <si>
-    <t>Loss const.</t>
-  </si>
-  <si>
     <t>d</t>
   </si>
   <si>
+    <t>Decay rate of A.</t>
+  </si>
+  <si>
     <t>decay constant of antibiotic</t>
   </si>
   <si>
-    <t>Decay rate of A.</t>
-  </si>
-  <si>
     <t>tau</t>
   </si>
   <si>
+    <t>Segregation rate.</t>
+  </si>
+  <si>
     <t>segregation rate</t>
   </si>
   <si>
-    <t>Segregation rate.</t>
-  </si>
-  <si>
     <t>gammaDR</t>
   </si>
   <si>
     <t>ml/cells/h</t>
   </si>
   <si>
-    <t>transfer rate D -&gt; R</t>
-  </si>
-  <si>
     <t>Transf. rate D-&gt;R</t>
   </si>
   <si>
-    <t>gammaTR</t>
-  </si>
-  <si>
-    <t>transfer rate T -&gt; R</t>
+    <t>transfer rate of plasmid from D to R</t>
+  </si>
+  <si>
+    <t>multTR</t>
+  </si>
+  <si>
+    <t>-</t>
   </si>
   <si>
     <t>Transf. rate T-&gt;R</t>
   </si>
   <si>
+    <t>controls plasmid transfer from T to R; gammaTR= multTR * gammaDR</t>
+  </si>
+  <si>
     <t>aD</t>
   </si>
   <si>
-    <t>-</t>
-  </si>
-  <si>
     <t>empirical par.</t>
   </si>
   <si>
@@ -195,7 +195,7 @@
     <t>fun</t>
   </si>
   <si>
-    <t>growth rate under antibiotic treatment</t>
+    <t>growth rate under possible antibiotic treatment</t>
   </si>
   <si>
     <t>fk</t>
@@ -270,7 +270,7 @@
     <t>fun(A,z,aD,bD,pD,qD) * D + fun(A,z,aT,bT,pT,qT) * T</t>
   </si>
   <si>
-    <t>-gammaDR * D - gammaTR * T</t>
+    <t>-gammaDR * D - (gammaDR * multTR) * T</t>
   </si>
   <si>
     <t>fun(A,z,aT,bT,pT,qT) * T</t>
@@ -282,7 +282,7 @@
     <t>-fun(A,z,aT,bT,pT,qT) * T</t>
   </si>
   <si>
-    <t>gammaDR * D + gammaTR * T</t>
+    <t>gammaDR * D + (gammaDR * multTR) * T</t>
   </si>
 </sst>
 </file>
@@ -482,8 +482,8 @@
   </sheetPr>
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E12" activeCellId="0" sqref="E12"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C18" activeCellId="0" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -632,10 +632,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="28.9081632653061"/>
-    <col collapsed="false" hidden="false" max="7" min="4" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="15.7857142857143"/>
+    <col collapsed="false" hidden="false" max="5" min="1" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="7" min="6" style="0" width="15.7857142857143"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="57.1530612244898"/>
     <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
@@ -647,22 +646,22 @@
         <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="3" t="s">
         <v>2</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -672,20 +671,20 @@
       <c r="B2" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="C2" s="2" t="n">
+        <v>3430000000</v>
+      </c>
+      <c r="D2" s="2" t="n">
+        <v>1720000000</v>
+      </c>
+      <c r="E2" s="2" t="n">
+        <v>6860000000</v>
+      </c>
+      <c r="F2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G2" s="0" t="s">
         <v>23</v>
-      </c>
-      <c r="D2" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="E2" s="2" t="n">
-        <v>3430000000</v>
-      </c>
-      <c r="F2" s="2" t="n">
-        <v>1720000000</v>
-      </c>
-      <c r="G2" s="2" t="n">
-        <v>6860000000</v>
       </c>
       <c r="H2" s="0" t="s">
         <v>24</v>
@@ -698,20 +697,20 @@
       <c r="B3" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="C3" s="0" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="D3" s="2" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="E3" s="2" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="F3" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G3" s="0" t="s">
         <v>27</v>
-      </c>
-      <c r="D3" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="E3" s="0" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="F3" s="2" t="n">
-        <v>0.05</v>
-      </c>
-      <c r="G3" s="2" t="n">
-        <v>0.2</v>
       </c>
       <c r="H3" s="0" t="s">
         <v>28</v>
@@ -724,20 +723,20 @@
       <c r="B4" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="C4" s="0" t="s">
+      <c r="C4" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D4" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E4" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F4" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G4" s="0" t="s">
         <v>30</v>
-      </c>
-      <c r="D4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="E4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="F4" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="G4" s="2" t="n">
-        <v>0</v>
       </c>
       <c r="H4" s="0" t="s">
         <v>31</v>
@@ -750,20 +749,20 @@
       <c r="B5" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="C5" s="0" t="s">
+      <c r="C5" s="2" t="n">
+        <v>5E-006</v>
+      </c>
+      <c r="D5" s="2" t="n">
+        <v>2.5E-006</v>
+      </c>
+      <c r="E5" s="2" t="n">
+        <v>1E-005</v>
+      </c>
+      <c r="F5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G5" s="0" t="s">
         <v>33</v>
-      </c>
-      <c r="D5" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="E5" s="2" t="n">
-        <v>5E-006</v>
-      </c>
-      <c r="F5" s="2" t="n">
-        <v>2.5E-006</v>
-      </c>
-      <c r="G5" s="2" t="n">
-        <v>1E-005</v>
       </c>
       <c r="H5" s="0" t="s">
         <v>34</v>
@@ -776,20 +775,20 @@
       <c r="B6" s="0" t="s">
         <v>36</v>
       </c>
-      <c r="C6" s="0" t="s">
+      <c r="C6" s="2" t="n">
+        <v>1.1E-011</v>
+      </c>
+      <c r="D6" s="2" t="n">
+        <v>5.5E-012</v>
+      </c>
+      <c r="E6" s="2" t="n">
+        <v>2.2E-011</v>
+      </c>
+      <c r="F6" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G6" s="0" t="s">
         <v>37</v>
-      </c>
-      <c r="D6" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="E6" s="2" t="n">
-        <v>1.1E-011</v>
-      </c>
-      <c r="F6" s="2" t="n">
-        <v>5.5E-012</v>
-      </c>
-      <c r="G6" s="2" t="n">
-        <v>2.2E-011</v>
       </c>
       <c r="H6" s="0" t="s">
         <v>38</v>
@@ -800,51 +799,51 @@
         <v>39</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="C7" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="D7" s="0" t="n">
+        <v>40</v>
+      </c>
+      <c r="C7" s="2" t="n">
+        <v>1.1E-011</v>
+      </c>
+      <c r="D7" s="2" t="n">
+        <v>5.5E-012</v>
+      </c>
+      <c r="E7" s="2" t="n">
+        <v>2.2E-011</v>
+      </c>
+      <c r="F7" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="E7" s="2" t="n">
-        <v>1.1E-011</v>
-      </c>
-      <c r="F7" s="2" t="n">
-        <v>5.5E-012</v>
-      </c>
-      <c r="G7" s="2" t="n">
-        <v>2.2E-011</v>
+      <c r="G7" s="0" t="s">
+        <v>41</v>
       </c>
       <c r="H7" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>43</v>
-      </c>
-      <c r="C8" s="0" t="s">
-        <v>44</v>
+        <v>40</v>
+      </c>
+      <c r="C8" s="0" t="n">
+        <v>0.22</v>
       </c>
       <c r="D8" s="0" t="n">
-        <v>0</v>
+        <v>0.22</v>
       </c>
       <c r="E8" s="0" t="n">
         <v>0.22</v>
       </c>
       <c r="F8" s="0" t="n">
-        <v>0.22</v>
-      </c>
-      <c r="G8" s="0" t="n">
-        <v>0.22</v>
+        <v>0</v>
+      </c>
+      <c r="G8" s="0" t="s">
+        <v>43</v>
       </c>
       <c r="H8" s="0" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -852,25 +851,25 @@
         <v>45</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>43</v>
-      </c>
-      <c r="C9" s="0" t="s">
-        <v>44</v>
+        <v>40</v>
+      </c>
+      <c r="C9" s="0" t="n">
+        <v>0.1</v>
       </c>
       <c r="D9" s="0" t="n">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="E9" s="0" t="n">
         <v>0.1</v>
       </c>
       <c r="F9" s="0" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="G9" s="0" t="n">
-        <v>0.1</v>
+        <v>0</v>
+      </c>
+      <c r="G9" s="0" t="s">
+        <v>45</v>
       </c>
       <c r="H9" s="0" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -878,25 +877,25 @@
         <v>46</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>43</v>
-      </c>
-      <c r="C10" s="0" t="s">
-        <v>44</v>
+        <v>40</v>
+      </c>
+      <c r="C10" s="0" t="n">
+        <v>23.42</v>
       </c>
       <c r="D10" s="0" t="n">
-        <v>0</v>
+        <v>23.42</v>
       </c>
       <c r="E10" s="0" t="n">
         <v>23.42</v>
       </c>
       <c r="F10" s="0" t="n">
-        <v>23.42</v>
-      </c>
-      <c r="G10" s="0" t="n">
-        <v>23.42</v>
+        <v>0</v>
+      </c>
+      <c r="G10" s="0" t="s">
+        <v>46</v>
       </c>
       <c r="H10" s="0" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -904,25 +903,25 @@
         <v>47</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>43</v>
-      </c>
-      <c r="C11" s="0" t="s">
-        <v>44</v>
+        <v>40</v>
+      </c>
+      <c r="C11" s="0" t="n">
+        <v>4.52</v>
       </c>
       <c r="D11" s="0" t="n">
-        <v>0</v>
+        <v>4.52</v>
       </c>
       <c r="E11" s="0" t="n">
         <v>4.52</v>
       </c>
       <c r="F11" s="0" t="n">
-        <v>4.52</v>
-      </c>
-      <c r="G11" s="0" t="n">
-        <v>4.52</v>
+        <v>0</v>
+      </c>
+      <c r="G11" s="0" t="s">
+        <v>47</v>
       </c>
       <c r="H11" s="0" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -930,25 +929,25 @@
         <v>48</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>43</v>
-      </c>
-      <c r="C12" s="0" t="s">
-        <v>44</v>
+        <v>40</v>
+      </c>
+      <c r="C12" s="0" t="n">
+        <v>0.22</v>
       </c>
       <c r="D12" s="0" t="n">
-        <v>0</v>
+        <v>0.22</v>
       </c>
       <c r="E12" s="0" t="n">
         <v>0.22</v>
       </c>
       <c r="F12" s="0" t="n">
-        <v>0.22</v>
-      </c>
-      <c r="G12" s="0" t="n">
-        <v>0.22</v>
+        <v>0</v>
+      </c>
+      <c r="G12" s="0" t="s">
+        <v>48</v>
       </c>
       <c r="H12" s="0" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -956,25 +955,25 @@
         <v>49</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>43</v>
-      </c>
-      <c r="C13" s="0" t="s">
-        <v>44</v>
+        <v>40</v>
+      </c>
+      <c r="C13" s="0" t="n">
+        <v>0.14</v>
       </c>
       <c r="D13" s="0" t="n">
-        <v>0</v>
+        <v>0.14</v>
       </c>
       <c r="E13" s="0" t="n">
         <v>0.14</v>
       </c>
       <c r="F13" s="0" t="n">
-        <v>0.14</v>
-      </c>
-      <c r="G13" s="0" t="n">
-        <v>0.14</v>
+        <v>0</v>
+      </c>
+      <c r="G13" s="0" t="s">
+        <v>49</v>
       </c>
       <c r="H13" s="0" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -982,25 +981,25 @@
         <v>50</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>43</v>
-      </c>
-      <c r="C14" s="0" t="s">
-        <v>44</v>
+        <v>40</v>
+      </c>
+      <c r="C14" s="0" t="n">
+        <v>29.6</v>
       </c>
       <c r="D14" s="0" t="n">
-        <v>0</v>
+        <v>29.6</v>
       </c>
       <c r="E14" s="0" t="n">
         <v>29.6</v>
       </c>
       <c r="F14" s="0" t="n">
-        <v>29.6</v>
-      </c>
-      <c r="G14" s="0" t="n">
-        <v>29.6</v>
+        <v>0</v>
+      </c>
+      <c r="G14" s="0" t="s">
+        <v>50</v>
       </c>
       <c r="H14" s="0" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1008,25 +1007,25 @@
         <v>51</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>43</v>
-      </c>
-      <c r="C15" s="0" t="s">
-        <v>44</v>
+        <v>40</v>
+      </c>
+      <c r="C15" s="0" t="n">
+        <v>0.73</v>
       </c>
       <c r="D15" s="0" t="n">
-        <v>0</v>
+        <v>0.73</v>
       </c>
       <c r="E15" s="0" t="n">
         <v>0.73</v>
       </c>
       <c r="F15" s="0" t="n">
-        <v>0.73</v>
-      </c>
-      <c r="G15" s="0" t="n">
-        <v>0.73</v>
+        <v>0</v>
+      </c>
+      <c r="G15" s="0" t="s">
+        <v>51</v>
       </c>
       <c r="H15" s="0" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1034,25 +1033,25 @@
         <v>52</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>43</v>
-      </c>
-      <c r="C16" s="0" t="s">
-        <v>44</v>
+        <v>40</v>
+      </c>
+      <c r="C16" s="0" t="n">
+        <v>0.24</v>
       </c>
       <c r="D16" s="0" t="n">
-        <v>0</v>
+        <v>0.24</v>
       </c>
       <c r="E16" s="0" t="n">
         <v>0.24</v>
       </c>
       <c r="F16" s="0" t="n">
-        <v>0.24</v>
-      </c>
-      <c r="G16" s="0" t="n">
-        <v>0.24</v>
+        <v>0</v>
+      </c>
+      <c r="G16" s="0" t="s">
+        <v>52</v>
       </c>
       <c r="H16" s="0" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1060,25 +1059,25 @@
         <v>53</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>43</v>
-      </c>
-      <c r="C17" s="0" t="s">
-        <v>44</v>
+        <v>40</v>
+      </c>
+      <c r="C17" s="0" t="n">
+        <v>0.08</v>
       </c>
       <c r="D17" s="0" t="n">
-        <v>0</v>
+        <v>0.08</v>
       </c>
       <c r="E17" s="0" t="n">
         <v>0.08</v>
       </c>
       <c r="F17" s="0" t="n">
-        <v>0.08</v>
-      </c>
-      <c r="G17" s="0" t="n">
-        <v>0.08</v>
+        <v>0</v>
+      </c>
+      <c r="G17" s="0" t="s">
+        <v>53</v>
       </c>
       <c r="H17" s="0" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1086,25 +1085,25 @@
         <v>54</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>43</v>
-      </c>
-      <c r="C18" s="0" t="s">
-        <v>44</v>
+        <v>40</v>
+      </c>
+      <c r="C18" s="0" t="n">
+        <v>25.19</v>
       </c>
       <c r="D18" s="0" t="n">
-        <v>0</v>
+        <v>25.19</v>
       </c>
       <c r="E18" s="0" t="n">
         <v>25.19</v>
       </c>
       <c r="F18" s="0" t="n">
-        <v>25.19</v>
-      </c>
-      <c r="G18" s="0" t="n">
-        <v>25.19</v>
+        <v>0</v>
+      </c>
+      <c r="G18" s="0" t="s">
+        <v>54</v>
       </c>
       <c r="H18" s="0" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1112,25 +1111,25 @@
         <v>55</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>43</v>
-      </c>
-      <c r="C19" s="0" t="s">
-        <v>44</v>
+        <v>40</v>
+      </c>
+      <c r="C19" s="0" t="n">
+        <v>4.15</v>
       </c>
       <c r="D19" s="0" t="n">
-        <v>0</v>
+        <v>4.15</v>
       </c>
       <c r="E19" s="0" t="n">
         <v>4.15</v>
       </c>
       <c r="F19" s="0" t="n">
-        <v>4.15</v>
-      </c>
-      <c r="G19" s="0" t="n">
-        <v>4.15</v>
+        <v>0</v>
+      </c>
+      <c r="G19" s="0" t="s">
+        <v>55</v>
       </c>
       <c r="H19" s="0" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1138,25 +1137,25 @@
         <v>56</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>43</v>
-      </c>
-      <c r="C20" s="0" t="s">
-        <v>44</v>
+        <v>40</v>
+      </c>
+      <c r="C20" s="0" t="n">
+        <v>0.5</v>
       </c>
       <c r="D20" s="0" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="E20" s="0" t="n">
         <v>0.5</v>
       </c>
       <c r="F20" s="0" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="G20" s="0" t="n">
-        <v>0.5</v>
+        <v>0</v>
+      </c>
+      <c r="G20" s="0" t="s">
+        <v>56</v>
       </c>
       <c r="H20" s="0" t="s">
-        <v>56</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -1178,13 +1177,13 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F9" activeCellId="0" sqref="F9"/>
+      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="2" min="1" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="34.9081632653061"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="47.5867346938776"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="6.44387755102041"/>
     <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="11.5204081632653"/>
   </cols>
@@ -1205,7 +1204,7 @@
         <v>57</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C2" s="0" t="s">
         <v>58</v>
@@ -1216,7 +1215,7 @@
         <v>59</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C3" s="0" t="s">
         <v>60</v>
@@ -1271,7 +1270,7 @@
         <v>62</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C2" s="0" t="s">
         <v>63</v>
@@ -1354,8 +1353,8 @@
   </sheetPr>
   <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C13" activeCellId="0" sqref="C13"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C14" activeCellId="0" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>

</xml_diff>

<commit_message>
ENH: Re-structured equations of example model (unchanged model behaviour)
</commit_message>
<xml_diff>
--- a/inst/examples/DRT/model.xlsx
+++ b/inst/examples/DRT/model.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="196" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="196" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="vars" sheetId="1" state="visible" r:id="rId2"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="93">
   <si>
     <t>name</t>
   </si>
@@ -207,30 +207,57 @@
     <t>expression</t>
   </si>
   <si>
-    <t>growth</t>
+    <t>growthD</t>
+  </si>
+  <si>
+    <t>cells/h</t>
+  </si>
+  <si>
+    <t>growth of donor</t>
+  </si>
+  <si>
+    <t>fk(K,D,R,T) * fun(A,z,aD,bD,pD,qD) * D</t>
+  </si>
+  <si>
+    <t>growthR</t>
+  </si>
+  <si>
+    <t>growth of recipient</t>
+  </si>
+  <si>
+    <t>fk(K,D,R,T) * fun(A,z,aR,bR,pR,qR) * R</t>
+  </si>
+  <si>
+    <t>growthT</t>
+  </si>
+  <si>
+    <t>growth of transconjugant</t>
+  </si>
+  <si>
+    <t>fk(K,D,R,T) * fun(A,z,aT,bT,pT,qT) * T</t>
+  </si>
+  <si>
+    <t>predation</t>
+  </si>
+  <si>
+    <t>common rate const. for all spec.</t>
+  </si>
+  <si>
+    <t>conjug</t>
+  </si>
+  <si>
+    <t>conjugation</t>
+  </si>
+  <si>
+    <t>fk(K,D,R,T) * R * (gammaDR * D + (gammaDR * multTR) * T)</t>
+  </si>
+  <si>
+    <t>segrLoss</t>
   </si>
   <si>
     <t>common term for all species</t>
   </si>
   <si>
-    <t>fk(K,D,R,T)</t>
-  </si>
-  <si>
-    <t>predation</t>
-  </si>
-  <si>
-    <t>common rate const. for all spec.</t>
-  </si>
-  <si>
-    <t>conjug</t>
-  </si>
-  <si>
-    <t>fk(K,D,R,T) * R</t>
-  </si>
-  <si>
-    <t>segrLoss</t>
-  </si>
-  <si>
     <t>fk(K,D,R,T) * tau</t>
   </si>
   <si>
@@ -252,7 +279,7 @@
     <t>-1</t>
   </si>
   <si>
-    <t>fun(A,z,aD,bD,pD,qD) * D</t>
+    <t>1</t>
   </si>
   <si>
     <t>-D</t>
@@ -261,28 +288,16 @@
     <t>-fun(A,z,aD,bD,pD,qD) * D</t>
   </si>
   <si>
-    <t>fun(A,z,aR,bR,pR,qR) * R</t>
-  </si>
-  <si>
     <t>-R</t>
   </si>
   <si>
     <t>fun(A,z,aD,bD,pD,qD) * D + fun(A,z,aT,bT,pT,qT) * T</t>
   </si>
   <si>
-    <t>-gammaDR * D - (gammaDR * multTR) * T</t>
-  </si>
-  <si>
-    <t>fun(A,z,aT,bT,pT,qT) * T</t>
-  </si>
-  <si>
     <t>-T</t>
   </si>
   <si>
     <t>-fun(A,z,aT,bT,pT,qT) * T</t>
-  </si>
-  <si>
-    <t>gammaDR * D + (gammaDR * multTR) * T</t>
   </si>
 </sst>
 </file>
@@ -294,7 +309,7 @@
     <numFmt numFmtId="165" formatCode="0.00E+000"/>
     <numFmt numFmtId="166" formatCode="@"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -317,10 +332,16 @@
       <family val="0"/>
     </font>
     <font>
+      <sz val="10"/>
+      <name val="Ubuntu Mono"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
       <b val="true"/>
       <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
+      <name val="Ubuntu Mono"/>
+      <family val="0"/>
       <charset val="1"/>
     </font>
   </fonts>
@@ -378,28 +399,32 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="166" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -482,129 +507,129 @@
   </sheetPr>
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C18" activeCellId="0" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="24.3520408163265"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="1" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="24.3520408163265"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="1" width="11.5204081632653"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="C2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E2" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="F2" s="0" t="n">
+      <c r="D2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2" s="1" t="n">
         <v>2.5</v>
       </c>
-      <c r="G2" s="0" t="s">
+      <c r="G2" s="1" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="C3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="2" t="n">
+      <c r="D3" s="3" t="n">
         <v>100000</v>
       </c>
-      <c r="E3" s="2" t="n">
+      <c r="E3" s="3" t="n">
         <v>100000</v>
       </c>
-      <c r="F3" s="2" t="n">
+      <c r="F3" s="3" t="n">
         <v>100000</v>
       </c>
-      <c r="G3" s="0" t="s">
+      <c r="G3" s="1" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="0" t="s">
+      <c r="C4" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D4" s="2" t="n">
+      <c r="D4" s="3" t="n">
         <v>100000</v>
       </c>
-      <c r="E4" s="2" t="n">
+      <c r="E4" s="3" t="n">
         <v>100000</v>
       </c>
-      <c r="F4" s="2" t="n">
+      <c r="F4" s="3" t="n">
         <v>100000</v>
       </c>
-      <c r="G4" s="0" t="s">
+      <c r="G4" s="1" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="A5" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="B5" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="0" t="s">
+      <c r="C5" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D5" s="0" t="n">
+      <c r="D5" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="E5" s="0" t="n">
+      <c r="E5" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="F5" s="0" t="n">
+      <c r="F5" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="G5" s="0" t="s">
+      <c r="G5" s="1" t="s">
         <v>20</v>
       </c>
     </row>
@@ -627,534 +652,534 @@
   <dimension ref="A1:H20"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H21" activeCellId="0" sqref="H21"/>
+      <selection pane="topLeft" activeCell="B30" activeCellId="0" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="5" min="1" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="7" min="6" style="0" width="15.7857142857143"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="57.1530612244898"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="5" min="1" style="1" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="7" min="6" style="1" width="15.7857142857143"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="57.1530612244898"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="1" width="11.5204081632653"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="3" t="s">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="4" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="2" t="n">
+      <c r="C2" s="3" t="n">
         <v>3430000000</v>
       </c>
-      <c r="D2" s="2" t="n">
+      <c r="D2" s="3" t="n">
         <v>1720000000</v>
       </c>
-      <c r="E2" s="2" t="n">
+      <c r="E2" s="3" t="n">
         <v>6860000000</v>
       </c>
-      <c r="F2" s="0" t="n">
+      <c r="F2" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="G2" s="0" t="s">
+      <c r="G2" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="H2" s="0" t="s">
+      <c r="H2" s="1" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C3" s="0" t="n">
+      <c r="C3" s="1" t="n">
         <v>0.1</v>
       </c>
-      <c r="D3" s="2" t="n">
+      <c r="D3" s="3" t="n">
         <v>0.05</v>
       </c>
-      <c r="E3" s="2" t="n">
+      <c r="E3" s="3" t="n">
         <v>0.2</v>
       </c>
-      <c r="F3" s="0" t="n">
+      <c r="F3" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="G3" s="0" t="s">
+      <c r="G3" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="H3" s="0" t="s">
+      <c r="H3" s="1" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="D4" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E4" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F4" s="0" t="n">
+      <c r="C4" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D4" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E4" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F4" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="G4" s="0" t="s">
+      <c r="G4" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="H4" s="0" t="s">
+      <c r="H4" s="1" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="A5" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="B5" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C5" s="2" t="n">
+      <c r="C5" s="3" t="n">
         <v>5E-006</v>
       </c>
-      <c r="D5" s="2" t="n">
+      <c r="D5" s="3" t="n">
         <v>2.5E-006</v>
       </c>
-      <c r="E5" s="2" t="n">
+      <c r="E5" s="3" t="n">
         <v>1E-005</v>
       </c>
-      <c r="F5" s="0" t="n">
+      <c r="F5" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="G5" s="0" t="s">
+      <c r="G5" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="H5" s="0" t="s">
+      <c r="H5" s="1" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+      <c r="A6" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B6" s="0" t="s">
+      <c r="B6" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C6" s="2" t="n">
+      <c r="C6" s="3" t="n">
         <v>1.1E-011</v>
       </c>
-      <c r="D6" s="2" t="n">
+      <c r="D6" s="3" t="n">
         <v>5.5E-012</v>
       </c>
-      <c r="E6" s="2" t="n">
+      <c r="E6" s="3" t="n">
         <v>2.2E-011</v>
       </c>
-      <c r="F6" s="0" t="n">
+      <c r="F6" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="G6" s="0" t="s">
+      <c r="G6" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="H6" s="0" t="s">
+      <c r="H6" s="1" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+      <c r="A7" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B7" s="0" t="s">
+      <c r="B7" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C7" s="2" t="n">
+      <c r="C7" s="3" t="n">
         <v>1.1E-011</v>
       </c>
-      <c r="D7" s="2" t="n">
+      <c r="D7" s="3" t="n">
         <v>5.5E-012</v>
       </c>
-      <c r="E7" s="2" t="n">
+      <c r="E7" s="3" t="n">
         <v>2.2E-011</v>
       </c>
-      <c r="F7" s="0" t="n">
+      <c r="F7" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="G7" s="0" t="s">
+      <c r="G7" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="H7" s="0" t="s">
+      <c r="H7" s="1" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
+      <c r="A8" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B8" s="0" t="s">
+      <c r="B8" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C8" s="0" t="n">
+      <c r="C8" s="1" t="n">
         <v>0.22</v>
       </c>
-      <c r="D8" s="0" t="n">
+      <c r="D8" s="1" t="n">
         <v>0.22</v>
       </c>
-      <c r="E8" s="0" t="n">
+      <c r="E8" s="1" t="n">
         <v>0.22</v>
       </c>
-      <c r="F8" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="G8" s="0" t="s">
+      <c r="F8" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="G8" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="H8" s="0" t="s">
+      <c r="H8" s="1" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
+      <c r="A9" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B9" s="0" t="s">
+      <c r="B9" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C9" s="0" t="n">
+      <c r="C9" s="1" t="n">
         <v>0.1</v>
       </c>
-      <c r="D9" s="0" t="n">
+      <c r="D9" s="1" t="n">
         <v>0.1</v>
       </c>
-      <c r="E9" s="0" t="n">
+      <c r="E9" s="1" t="n">
         <v>0.1</v>
       </c>
-      <c r="F9" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="G9" s="0" t="s">
+      <c r="F9" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="G9" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="H9" s="0" t="s">
+      <c r="H9" s="1" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
+      <c r="A10" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B10" s="0" t="s">
+      <c r="B10" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C10" s="0" t="n">
+      <c r="C10" s="1" t="n">
         <v>23.42</v>
       </c>
-      <c r="D10" s="0" t="n">
+      <c r="D10" s="1" t="n">
         <v>23.42</v>
       </c>
-      <c r="E10" s="0" t="n">
+      <c r="E10" s="1" t="n">
         <v>23.42</v>
       </c>
-      <c r="F10" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="G10" s="0" t="s">
+      <c r="F10" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="G10" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="H10" s="0" t="s">
+      <c r="H10" s="1" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
+      <c r="A11" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B11" s="0" t="s">
+      <c r="B11" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C11" s="0" t="n">
+      <c r="C11" s="1" t="n">
         <v>4.52</v>
       </c>
-      <c r="D11" s="0" t="n">
+      <c r="D11" s="1" t="n">
         <v>4.52</v>
       </c>
-      <c r="E11" s="0" t="n">
+      <c r="E11" s="1" t="n">
         <v>4.52</v>
       </c>
-      <c r="F11" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="G11" s="0" t="s">
+      <c r="F11" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="G11" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="H11" s="0" t="s">
+      <c r="H11" s="1" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
+      <c r="A12" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B12" s="0" t="s">
+      <c r="B12" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C12" s="0" t="n">
+      <c r="C12" s="1" t="n">
         <v>0.22</v>
       </c>
-      <c r="D12" s="0" t="n">
+      <c r="D12" s="1" t="n">
         <v>0.22</v>
       </c>
-      <c r="E12" s="0" t="n">
+      <c r="E12" s="1" t="n">
         <v>0.22</v>
       </c>
-      <c r="F12" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="G12" s="0" t="s">
+      <c r="F12" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="G12" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="H12" s="0" t="s">
+      <c r="H12" s="1" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
+      <c r="A13" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B13" s="0" t="s">
+      <c r="B13" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C13" s="0" t="n">
+      <c r="C13" s="1" t="n">
         <v>0.14</v>
       </c>
-      <c r="D13" s="0" t="n">
+      <c r="D13" s="1" t="n">
         <v>0.14</v>
       </c>
-      <c r="E13" s="0" t="n">
+      <c r="E13" s="1" t="n">
         <v>0.14</v>
       </c>
-      <c r="F13" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="G13" s="0" t="s">
+      <c r="F13" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="G13" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="H13" s="0" t="s">
+      <c r="H13" s="1" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
+      <c r="A14" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="B14" s="0" t="s">
+      <c r="B14" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C14" s="0" t="n">
+      <c r="C14" s="1" t="n">
         <v>29.6</v>
       </c>
-      <c r="D14" s="0" t="n">
+      <c r="D14" s="1" t="n">
         <v>29.6</v>
       </c>
-      <c r="E14" s="0" t="n">
+      <c r="E14" s="1" t="n">
         <v>29.6</v>
       </c>
-      <c r="F14" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="G14" s="0" t="s">
+      <c r="F14" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="G14" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="H14" s="0" t="s">
+      <c r="H14" s="1" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="s">
+      <c r="A15" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B15" s="0" t="s">
+      <c r="B15" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C15" s="0" t="n">
+      <c r="C15" s="1" t="n">
         <v>0.73</v>
       </c>
-      <c r="D15" s="0" t="n">
+      <c r="D15" s="1" t="n">
         <v>0.73</v>
       </c>
-      <c r="E15" s="0" t="n">
+      <c r="E15" s="1" t="n">
         <v>0.73</v>
       </c>
-      <c r="F15" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="G15" s="0" t="s">
+      <c r="F15" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="G15" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="H15" s="0" t="s">
+      <c r="H15" s="1" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="s">
+      <c r="A16" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="B16" s="0" t="s">
+      <c r="B16" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C16" s="0" t="n">
+      <c r="C16" s="1" t="n">
         <v>0.24</v>
       </c>
-      <c r="D16" s="0" t="n">
+      <c r="D16" s="1" t="n">
         <v>0.24</v>
       </c>
-      <c r="E16" s="0" t="n">
+      <c r="E16" s="1" t="n">
         <v>0.24</v>
       </c>
-      <c r="F16" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="G16" s="0" t="s">
+      <c r="F16" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="G16" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="H16" s="0" t="s">
+      <c r="H16" s="1" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="s">
+      <c r="A17" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B17" s="0" t="s">
+      <c r="B17" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C17" s="0" t="n">
+      <c r="C17" s="1" t="n">
         <v>0.08</v>
       </c>
-      <c r="D17" s="0" t="n">
+      <c r="D17" s="1" t="n">
         <v>0.08</v>
       </c>
-      <c r="E17" s="0" t="n">
+      <c r="E17" s="1" t="n">
         <v>0.08</v>
       </c>
-      <c r="F17" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="G17" s="0" t="s">
+      <c r="F17" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="G17" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="H17" s="0" t="s">
+      <c r="H17" s="1" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="s">
+      <c r="A18" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="B18" s="0" t="s">
+      <c r="B18" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C18" s="0" t="n">
+      <c r="C18" s="1" t="n">
         <v>25.19</v>
       </c>
-      <c r="D18" s="0" t="n">
+      <c r="D18" s="1" t="n">
         <v>25.19</v>
       </c>
-      <c r="E18" s="0" t="n">
+      <c r="E18" s="1" t="n">
         <v>25.19</v>
       </c>
-      <c r="F18" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="G18" s="0" t="s">
+      <c r="F18" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="G18" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="H18" s="0" t="s">
+      <c r="H18" s="1" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="s">
+      <c r="A19" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B19" s="0" t="s">
+      <c r="B19" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C19" s="0" t="n">
+      <c r="C19" s="1" t="n">
         <v>4.15</v>
       </c>
-      <c r="D19" s="0" t="n">
+      <c r="D19" s="1" t="n">
         <v>4.15</v>
       </c>
-      <c r="E19" s="0" t="n">
+      <c r="E19" s="1" t="n">
         <v>4.15</v>
       </c>
-      <c r="F19" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="G19" s="0" t="s">
+      <c r="F19" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="G19" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="H19" s="0" t="s">
+      <c r="H19" s="1" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="s">
+      <c r="A20" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B20" s="0" t="s">
+      <c r="B20" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C20" s="0" t="n">
+      <c r="C20" s="1" t="n">
         <v>0.5</v>
       </c>
-      <c r="D20" s="0" t="n">
+      <c r="D20" s="1" t="n">
         <v>0.5</v>
       </c>
-      <c r="E20" s="0" t="n">
+      <c r="E20" s="1" t="n">
         <v>0.5</v>
       </c>
-      <c r="F20" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="G20" s="0" t="s">
+      <c r="F20" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="G20" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="H20" s="0" t="s">
+      <c r="H20" s="1" t="s">
         <v>44</v>
       </c>
     </row>
@@ -1182,42 +1207,42 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="47.5867346938776"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="6.44387755102041"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="1" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="47.5867346938776"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="6.44387755102041"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="1" width="11.5204081632653"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="3" t="s">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="C2" s="1" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="C3" s="1" t="s">
         <v>60</v>
       </c>
     </row>
@@ -1237,102 +1262,130 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C13" activeCellId="0" sqref="C13"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="28.9081632653061"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.3418367346939"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="1" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="28.9081632653061"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="51.7040816326531"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="1" width="11.5204081632653"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="B2" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="C2" s="0" t="s">
+      <c r="B2" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="C2" s="1" t="s">
         <v>64</v>
       </c>
+      <c r="D2" s="1" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
-        <v>65</v>
-      </c>
-      <c r="B3" s="0" t="s">
+      <c r="A3" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C3" s="0" t="s">
-        <v>66</v>
-      </c>
-      <c r="D3" s="0" t="s">
+      <c r="C5" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
-        <v>67</v>
-      </c>
-      <c r="B4" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" s="0" t="s">
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="D4" s="0" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
-        <v>69</v>
-      </c>
-      <c r="B5" s="0" t="s">
+      <c r="C6" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C5" s="0" t="s">
-        <v>63</v>
-      </c>
-      <c r="D5" s="0" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
-        <v>71</v>
-      </c>
-      <c r="B6" s="0" t="s">
+      <c r="C7" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C6" s="0" t="s">
-        <v>72</v>
-      </c>
-      <c r="D6" s="0" t="s">
-        <v>73</v>
+      <c r="C8" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>82</v>
       </c>
     </row>
   </sheetData>
@@ -1354,157 +1407,157 @@
   <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C14" activeCellId="0" sqref="C14"/>
+      <selection pane="topLeft" activeCell="C26" activeCellId="0" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="43.5867346938776"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="1" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="48.3724489795918"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="1" width="11.5204081632653"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" s="0" t="s">
-        <v>71</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3" s="0" t="s">
-        <v>62</v>
-      </c>
-      <c r="C3" s="5" t="s">
+      <c r="C9" s="6" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" s="0" t="s">
-        <v>65</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5" s="0" t="s">
-        <v>69</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="B6" s="0" t="s">
-        <v>62</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="B7" s="0" t="s">
-        <v>65</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="B8" s="0" t="s">
-        <v>69</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="B9" s="0" t="s">
-        <v>67</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
+      <c r="C12" s="6" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="0" t="s">
-        <v>62</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="B11" s="0" t="s">
-        <v>65</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="B12" s="0" t="s">
-        <v>69</v>
-      </c>
-      <c r="C12" s="5" t="s">
+      <c r="B13" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C13" s="6" t="s">
         <v>86</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="B13" s="0" t="s">
-        <v>67</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>87</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ENH: Added columns 'tex' and 'html' to tables of example model as required by latest version of 'rodeo'
</commit_message>
<xml_diff>
--- a/inst/examples/DRT/model.xlsx
+++ b/inst/examples/DRT/model.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="196" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="184" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="vars" sheetId="1" state="visible" r:id="rId2"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="99">
   <si>
     <t>name</t>
   </si>
@@ -42,6 +42,12 @@
     <t>label</t>
   </si>
   <si>
+    <t>tex</t>
+  </si>
+  <si>
+    <t>html</t>
+  </si>
+  <si>
     <t>A</t>
   </si>
   <si>
@@ -138,6 +144,12 @@
     <t>transfer rate of plasmid from D to R</t>
   </si>
   <si>
+    <t>\Gamma_{DR}</t>
+  </si>
+  <si>
+    <t>&amp;Gamma;&lt;sub&gt;DR&lt;/sub&gt;</t>
+  </si>
+  <si>
     <t>multTR</t>
   </si>
   <si>
@@ -148,6 +160,12 @@
   </si>
   <si>
     <t>controls plasmid transfer from T to R; gammaTR= multTR * gammaDR</t>
+  </si>
+  <si>
+    <t>mult_{TR}</t>
+  </si>
+  <si>
+    <t>mult&lt;sub&gt;TR&lt;/sub&gt;</t>
   </si>
   <si>
     <t>aD</t>
@@ -505,10 +523,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C18" activeCellId="0" sqref="C18"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G21" activeCellId="0" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -540,16 +558,22 @@
       <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
+      <c r="H1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D2" s="1" t="n">
         <v>0</v>
@@ -561,18 +585,24 @@
         <v>2.5</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D3" s="3" t="n">
         <v>100000</v>
@@ -584,18 +614,24 @@
         <v>100000</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D4" s="3" t="n">
         <v>100000</v>
@@ -607,18 +643,24 @@
         <v>100000</v>
       </c>
       <c r="G4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I4" s="1" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D5" s="1" t="n">
         <v>1</v>
@@ -630,6 +672,12 @@
         <v>1</v>
       </c>
       <c r="G5" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I5" s="1" t="s">
         <v>20</v>
       </c>
     </row>
@@ -649,18 +697,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H20"/>
+  <dimension ref="A1:J20"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B30" activeCellId="0" sqref="B30"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I1" activeCellId="0" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="5" min="1" style="1" width="11.5204081632653"/>
     <col collapsed="false" hidden="false" max="7" min="6" style="1" width="15.7857142857143"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="57.1530612244898"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="1" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="63.9336734693878"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="22.0918367346939"/>
+    <col collapsed="false" hidden="false" max="1025" min="11" style="1" width="11.5204081632653"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -680,7 +730,7 @@
         <v>5</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="G1" s="4" t="s">
         <v>6</v>
@@ -688,13 +738,19 @@
       <c r="H1" s="4" t="s">
         <v>2</v>
       </c>
+      <c r="I1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C2" s="3" t="n">
         <v>3430000000</v>
@@ -709,18 +765,26 @@
         <v>1</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
+      </c>
+      <c r="I2" s="1" t="str">
+        <f aca="false">A2</f>
+        <v>K</v>
+      </c>
+      <c r="J2" s="1" t="str">
+        <f aca="false">A2</f>
+        <v>K</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C3" s="1" t="n">
         <v>0.1</v>
@@ -735,18 +799,26 @@
         <v>1</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
+      </c>
+      <c r="I3" s="1" t="str">
+        <f aca="false">A3</f>
+        <v>g</v>
+      </c>
+      <c r="J3" s="1" t="str">
+        <f aca="false">A3</f>
+        <v>g</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C4" s="1" t="n">
         <v>0</v>
@@ -761,18 +833,26 @@
         <v>1</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
+      </c>
+      <c r="I4" s="1" t="str">
+        <f aca="false">A4</f>
+        <v>d</v>
+      </c>
+      <c r="J4" s="1" t="str">
+        <f aca="false">A4</f>
+        <v>d</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C5" s="3" t="n">
         <v>5E-006</v>
@@ -787,18 +867,26 @@
         <v>1</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
+      </c>
+      <c r="I5" s="1" t="str">
+        <f aca="false">A5</f>
+        <v>tau</v>
+      </c>
+      <c r="J5" s="1" t="str">
+        <f aca="false">A5</f>
+        <v>tau</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C6" s="3" t="n">
         <v>1.1E-011</v>
@@ -813,18 +901,24 @@
         <v>1</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>38</v>
+        <v>40</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="C7" s="3" t="n">
         <v>1.1E-011</v>
@@ -839,18 +933,24 @@
         <v>1</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>42</v>
+        <v>46</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="C8" s="1" t="n">
         <v>0.22</v>
@@ -865,18 +965,26 @@
         <v>0</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>44</v>
+        <v>50</v>
+      </c>
+      <c r="I8" s="1" t="str">
+        <f aca="false">A8</f>
+        <v>aD</v>
+      </c>
+      <c r="J8" s="1" t="str">
+        <f aca="false">A8</f>
+        <v>aD</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="C9" s="1" t="n">
         <v>0.1</v>
@@ -891,18 +999,26 @@
         <v>0</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>44</v>
+        <v>50</v>
+      </c>
+      <c r="I9" s="1" t="str">
+        <f aca="false">A9</f>
+        <v>bD</v>
+      </c>
+      <c r="J9" s="1" t="str">
+        <f aca="false">A9</f>
+        <v>bD</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="C10" s="1" t="n">
         <v>23.42</v>
@@ -917,18 +1033,26 @@
         <v>0</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>44</v>
+        <v>50</v>
+      </c>
+      <c r="I10" s="1" t="str">
+        <f aca="false">A10</f>
+        <v>pD</v>
+      </c>
+      <c r="J10" s="1" t="str">
+        <f aca="false">A10</f>
+        <v>pD</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="C11" s="1" t="n">
         <v>4.52</v>
@@ -943,18 +1067,26 @@
         <v>0</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>44</v>
+        <v>50</v>
+      </c>
+      <c r="I11" s="1" t="str">
+        <f aca="false">A11</f>
+        <v>qD</v>
+      </c>
+      <c r="J11" s="1" t="str">
+        <f aca="false">A11</f>
+        <v>qD</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="C12" s="1" t="n">
         <v>0.22</v>
@@ -969,18 +1101,26 @@
         <v>0</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>44</v>
+        <v>50</v>
+      </c>
+      <c r="I12" s="1" t="str">
+        <f aca="false">A12</f>
+        <v>aR</v>
+      </c>
+      <c r="J12" s="1" t="str">
+        <f aca="false">A12</f>
+        <v>aR</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="C13" s="1" t="n">
         <v>0.14</v>
@@ -995,18 +1135,26 @@
         <v>0</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>44</v>
+        <v>50</v>
+      </c>
+      <c r="I13" s="1" t="str">
+        <f aca="false">A13</f>
+        <v>bR</v>
+      </c>
+      <c r="J13" s="1" t="str">
+        <f aca="false">A13</f>
+        <v>bR</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="C14" s="1" t="n">
         <v>29.6</v>
@@ -1021,18 +1169,26 @@
         <v>0</v>
       </c>
       <c r="G14" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="H14" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="H14" s="1" t="s">
-        <v>44</v>
+      <c r="I14" s="1" t="str">
+        <f aca="false">A14</f>
+        <v>pR</v>
+      </c>
+      <c r="J14" s="1" t="str">
+        <f aca="false">A14</f>
+        <v>pR</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="C15" s="1" t="n">
         <v>0.73</v>
@@ -1047,18 +1203,26 @@
         <v>0</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>44</v>
+        <v>50</v>
+      </c>
+      <c r="I15" s="1" t="str">
+        <f aca="false">A15</f>
+        <v>qR</v>
+      </c>
+      <c r="J15" s="1" t="str">
+        <f aca="false">A15</f>
+        <v>qR</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="C16" s="1" t="n">
         <v>0.24</v>
@@ -1073,18 +1237,26 @@
         <v>0</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>44</v>
+        <v>50</v>
+      </c>
+      <c r="I16" s="1" t="str">
+        <f aca="false">A16</f>
+        <v>aT</v>
+      </c>
+      <c r="J16" s="1" t="str">
+        <f aca="false">A16</f>
+        <v>aT</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="C17" s="1" t="n">
         <v>0.08</v>
@@ -1099,18 +1271,26 @@
         <v>0</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>44</v>
+        <v>50</v>
+      </c>
+      <c r="I17" s="1" t="str">
+        <f aca="false">A17</f>
+        <v>bT</v>
+      </c>
+      <c r="J17" s="1" t="str">
+        <f aca="false">A17</f>
+        <v>bT</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="C18" s="1" t="n">
         <v>25.19</v>
@@ -1125,18 +1305,26 @@
         <v>0</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>44</v>
+        <v>50</v>
+      </c>
+      <c r="I18" s="1" t="str">
+        <f aca="false">A18</f>
+        <v>pT</v>
+      </c>
+      <c r="J18" s="1" t="str">
+        <f aca="false">A18</f>
+        <v>pT</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="C19" s="1" t="n">
         <v>4.15</v>
@@ -1151,18 +1339,26 @@
         <v>0</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>44</v>
+        <v>50</v>
+      </c>
+      <c r="I19" s="1" t="str">
+        <f aca="false">A19</f>
+        <v>qT</v>
+      </c>
+      <c r="J19" s="1" t="str">
+        <f aca="false">A19</f>
+        <v>qT</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="C20" s="1" t="n">
         <v>0.5</v>
@@ -1177,10 +1373,18 @@
         <v>0</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>44</v>
+        <v>50</v>
+      </c>
+      <c r="I20" s="1" t="str">
+        <f aca="false">A20</f>
+        <v>z</v>
+      </c>
+      <c r="J20" s="1" t="str">
+        <f aca="false">A20</f>
+        <v>z</v>
       </c>
     </row>
   </sheetData>
@@ -1199,10 +1403,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E4" activeCellId="0" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1223,27 +1427,45 @@
       <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
+      <c r="D1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>58</v>
+        <v>64</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>60</v>
+        <v>66</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>65</v>
       </c>
     </row>
   </sheetData>
@@ -1264,8 +1486,8 @@
   </sheetPr>
   <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1287,105 +1509,105 @@
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>63</v>
-      </c>
       <c r="C4" s="1" t="s">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>73</v>
+        <v>79</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>77</v>
+        <v>83</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
     </row>
   </sheetData>
@@ -1406,7 +1628,7 @@
   </sheetPr>
   <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C26" activeCellId="0" sqref="C26"/>
     </sheetView>
   </sheetViews>
@@ -1419,145 +1641,145 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>83</v>
+        <v>89</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>77</v>
+        <v>83</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>88</v>
+        <v>94</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>89</v>
+        <v>95</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>77</v>
+        <v>83</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>90</v>
+        <v>96</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>69</v>
+        <v>75</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>91</v>
+        <v>97</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>77</v>
+        <v>83</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ENH: new mandatory fields in table of variables: 'rtol', 'atol', 'show', and 'mult'; stoichiometry matrix plotted as table
</commit_message>
<xml_diff>
--- a/inst/examples/DRT/model.xlsx
+++ b/inst/examples/DRT/model.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="184" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="184" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="vars" sheetId="1" state="visible" r:id="rId2"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="103">
   <si>
     <t>name</t>
   </si>
@@ -46,6 +46,18 @@
   </si>
   <si>
     <t>html</t>
+  </si>
+  <si>
+    <t>mult</t>
+  </si>
+  <si>
+    <t>show</t>
+  </si>
+  <si>
+    <t>rtol</t>
+  </si>
+  <si>
+    <t>atol</t>
   </si>
   <si>
     <t>A</t>
@@ -327,7 +339,7 @@
     <numFmt numFmtId="165" formatCode="0.00E+000"/>
     <numFmt numFmtId="166" formatCode="@"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -358,6 +370,14 @@
     <font>
       <b val="true"/>
       <sz val="10"/>
+      <name val="Ubuntu Mono"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
       <name val="Ubuntu Mono"/>
       <family val="0"/>
       <charset val="1"/>
@@ -417,7 +437,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -427,6 +447,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -523,10 +547,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I5"/>
+  <dimension ref="A1:M5"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G21" activeCellId="0" sqref="G21"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="M3" activeCellId="0" sqref="M3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -564,16 +588,28 @@
       <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
+      <c r="J1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="D2" s="1" t="n">
         <v>0</v>
@@ -585,82 +621,118 @@
         <v>2.5</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>9</v>
+        <v>13</v>
+      </c>
+      <c r="J2" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="K2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="L2" s="4" t="n">
+        <v>1E-006</v>
+      </c>
+      <c r="M2" s="4" t="n">
+        <v>1E-006</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D3" s="3" t="n">
+        <v>19</v>
+      </c>
+      <c r="D3" s="4" t="n">
         <v>100000</v>
       </c>
-      <c r="E3" s="3" t="n">
+      <c r="E3" s="4" t="n">
         <v>100000</v>
       </c>
-      <c r="F3" s="3" t="n">
+      <c r="F3" s="4" t="n">
         <v>100000</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>13</v>
+        <v>17</v>
+      </c>
+      <c r="J3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="K3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="L3" s="4" t="n">
+        <v>1E-006</v>
+      </c>
+      <c r="M3" s="4" t="n">
+        <v>1E-006</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D4" s="3" t="n">
+        <v>22</v>
+      </c>
+      <c r="D4" s="4" t="n">
         <v>100000</v>
       </c>
-      <c r="E4" s="3" t="n">
+      <c r="E4" s="4" t="n">
         <v>100000</v>
       </c>
-      <c r="F4" s="3" t="n">
+      <c r="F4" s="4" t="n">
         <v>100000</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>17</v>
+        <v>21</v>
+      </c>
+      <c r="J4" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="K4" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="L4" s="4" t="n">
+        <v>1E-006</v>
+      </c>
+      <c r="M4" s="4" t="n">
+        <v>1E-006</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="D5" s="1" t="n">
         <v>1</v>
@@ -672,13 +744,25 @@
         <v>1</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>20</v>
+        <v>24</v>
+      </c>
+      <c r="J5" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="K5" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="L5" s="4" t="n">
+        <v>1E-006</v>
+      </c>
+      <c r="M5" s="4" t="n">
+        <v>1E-006</v>
       </c>
     </row>
   </sheetData>
@@ -714,28 +798,28 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="4" t="s">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="G1" s="4" t="s">
+      <c r="F1" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H1" s="5" t="s">
         <v>2</v>
       </c>
       <c r="I1" s="2" t="s">
@@ -747,28 +831,28 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C2" s="3" t="n">
+        <v>18</v>
+      </c>
+      <c r="C2" s="4" t="n">
         <v>3430000000</v>
       </c>
-      <c r="D2" s="3" t="n">
+      <c r="D2" s="4" t="n">
         <v>1720000000</v>
       </c>
-      <c r="E2" s="3" t="n">
+      <c r="E2" s="4" t="n">
         <v>6860000000</v>
       </c>
       <c r="F2" s="1" t="n">
         <v>1</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="I2" s="1" t="str">
         <f aca="false">A2</f>
@@ -781,28 +865,28 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="C3" s="1" t="n">
         <v>0.1</v>
       </c>
-      <c r="D3" s="3" t="n">
+      <c r="D3" s="4" t="n">
         <v>0.05</v>
       </c>
-      <c r="E3" s="3" t="n">
+      <c r="E3" s="4" t="n">
         <v>0.2</v>
       </c>
       <c r="F3" s="1" t="n">
         <v>1</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="I3" s="1" t="str">
         <f aca="false">A3</f>
@@ -815,28 +899,28 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="C4" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="D4" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="E4" s="3" t="n">
+      <c r="D4" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="E4" s="4" t="n">
         <v>0</v>
       </c>
       <c r="F4" s="1" t="n">
         <v>1</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="I4" s="1" t="str">
         <f aca="false">A4</f>
@@ -849,28 +933,28 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C5" s="3" t="n">
+        <v>32</v>
+      </c>
+      <c r="C5" s="4" t="n">
         <v>5E-006</v>
       </c>
-      <c r="D5" s="3" t="n">
+      <c r="D5" s="4" t="n">
         <v>2.5E-006</v>
       </c>
-      <c r="E5" s="3" t="n">
+      <c r="E5" s="4" t="n">
         <v>1E-005</v>
       </c>
       <c r="F5" s="1" t="n">
         <v>1</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="I5" s="1" t="str">
         <f aca="false">A5</f>
@@ -883,74 +967,74 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="C6" s="3" t="n">
+        <v>42</v>
+      </c>
+      <c r="C6" s="4" t="n">
         <v>1.1E-011</v>
       </c>
-      <c r="D6" s="3" t="n">
+      <c r="D6" s="4" t="n">
         <v>5.5E-012</v>
       </c>
-      <c r="E6" s="3" t="n">
+      <c r="E6" s="4" t="n">
         <v>2.2E-011</v>
       </c>
       <c r="F6" s="1" t="n">
         <v>1</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="C7" s="3" t="n">
+        <v>48</v>
+      </c>
+      <c r="C7" s="4" t="n">
         <v>1.1E-011</v>
       </c>
-      <c r="D7" s="3" t="n">
+      <c r="D7" s="4" t="n">
         <v>5.5E-012</v>
       </c>
-      <c r="E7" s="3" t="n">
+      <c r="E7" s="4" t="n">
         <v>2.2E-011</v>
       </c>
       <c r="F7" s="1" t="n">
         <v>1</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="C8" s="1" t="n">
         <v>0.22</v>
@@ -965,10 +1049,10 @@
         <v>0</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="I8" s="1" t="str">
         <f aca="false">A8</f>
@@ -981,10 +1065,10 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="C9" s="1" t="n">
         <v>0.1</v>
@@ -999,10 +1083,10 @@
         <v>0</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="I9" s="1" t="str">
         <f aca="false">A9</f>
@@ -1015,10 +1099,10 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="C10" s="1" t="n">
         <v>23.42</v>
@@ -1033,10 +1117,10 @@
         <v>0</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="I10" s="1" t="str">
         <f aca="false">A10</f>
@@ -1049,10 +1133,10 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="C11" s="1" t="n">
         <v>4.52</v>
@@ -1067,10 +1151,10 @@
         <v>0</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="I11" s="1" t="str">
         <f aca="false">A11</f>
@@ -1083,10 +1167,10 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="C12" s="1" t="n">
         <v>0.22</v>
@@ -1101,10 +1185,10 @@
         <v>0</v>
       </c>
       <c r="G12" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="H12" s="1" t="s">
         <v>54</v>
-      </c>
-      <c r="H12" s="1" t="s">
-        <v>50</v>
       </c>
       <c r="I12" s="1" t="str">
         <f aca="false">A12</f>
@@ -1117,10 +1201,10 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="C13" s="1" t="n">
         <v>0.14</v>
@@ -1135,10 +1219,10 @@
         <v>0</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="I13" s="1" t="str">
         <f aca="false">A13</f>
@@ -1151,10 +1235,10 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="C14" s="1" t="n">
         <v>29.6</v>
@@ -1169,10 +1253,10 @@
         <v>0</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="I14" s="1" t="str">
         <f aca="false">A14</f>
@@ -1185,10 +1269,10 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="C15" s="1" t="n">
         <v>0.73</v>
@@ -1203,10 +1287,10 @@
         <v>0</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="I15" s="1" t="str">
         <f aca="false">A15</f>
@@ -1219,10 +1303,10 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="C16" s="1" t="n">
         <v>0.24</v>
@@ -1237,10 +1321,10 @@
         <v>0</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="I16" s="1" t="str">
         <f aca="false">A16</f>
@@ -1253,10 +1337,10 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="C17" s="1" t="n">
         <v>0.08</v>
@@ -1271,10 +1355,10 @@
         <v>0</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="I17" s="1" t="str">
         <f aca="false">A17</f>
@@ -1287,10 +1371,10 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="C18" s="1" t="n">
         <v>25.19</v>
@@ -1305,10 +1389,10 @@
         <v>0</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="I18" s="1" t="str">
         <f aca="false">A18</f>
@@ -1321,10 +1405,10 @@
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="C19" s="1" t="n">
         <v>4.15</v>
@@ -1339,10 +1423,10 @@
         <v>0</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="I19" s="1" t="str">
         <f aca="false">A19</f>
@@ -1355,10 +1439,10 @@
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="C20" s="1" t="n">
         <v>0.5</v>
@@ -1373,10 +1457,10 @@
         <v>0</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="I20" s="1" t="str">
         <f aca="false">A20</f>
@@ -1405,7 +1489,7 @@
   </sheetPr>
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E4" activeCellId="0" sqref="E4"/>
     </sheetView>
   </sheetViews>
@@ -1418,13 +1502,13 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="4" t="s">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="5" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
@@ -1436,36 +1520,36 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
     </row>
   </sheetData>
@@ -1509,105 +1593,105 @@
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
     </row>
   </sheetData>
@@ -1641,145 +1725,145 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>67</v>
+        <v>94</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>91</v>
+        <v>90</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>92</v>
+        <v>72</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>93</v>
+        <v>82</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>94</v>
+        <v>87</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>92</v>
+        <v>76</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>95</v>
+        <v>82</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>96</v>
+        <v>87</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>91</v>
+        <v>84</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>92</v>
+        <v>79</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>97</v>
+        <v>82</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="C12" s="6" t="s">
-        <v>98</v>
+        <v>87</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="C13" s="6" t="s">
-        <v>92</v>
+        <v>84</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>96</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ENH: Support for optional 'color' column in table of variables
</commit_message>
<xml_diff>
--- a/inst/examples/DRT/model.xlsx
+++ b/inst/examples/DRT/model.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="184" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="120" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="vars" sheetId="1" state="visible" r:id="rId2"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="108">
   <si>
     <t>name</t>
   </si>
@@ -60,6 +60,9 @@
     <t>atol</t>
   </si>
   <si>
+    <t>color</t>
+  </si>
+  <si>
     <t>A</t>
   </si>
   <si>
@@ -72,6 +75,9 @@
     <t>Antibiotic</t>
   </si>
   <si>
+    <t>black</t>
+  </si>
+  <si>
     <t>D</t>
   </si>
   <si>
@@ -84,6 +90,9 @@
     <t>Donors</t>
   </si>
   <si>
+    <t>indianred</t>
+  </si>
+  <si>
     <t>R</t>
   </si>
   <si>
@@ -93,6 +102,9 @@
     <t>Recipients</t>
   </si>
   <si>
+    <t>steelblue2</t>
+  </si>
+  <si>
     <t>T</t>
   </si>
   <si>
@@ -100,6 +112,9 @@
   </si>
   <si>
     <t>Transconj.</t>
+  </si>
+  <si>
+    <t>violet</t>
   </si>
   <si>
     <t>user</t>
@@ -547,10 +562,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M5"/>
+  <dimension ref="A1:N5"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M3" activeCellId="0" sqref="M3"/>
+      <selection pane="topLeft" activeCell="N6" activeCellId="0" sqref="N6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -600,16 +615,19 @@
       <c r="M1" s="3" t="s">
         <v>12</v>
       </c>
+      <c r="N1" s="3" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D2" s="1" t="n">
         <v>0</v>
@@ -621,13 +639,13 @@
         <v>2.5</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="J2" s="1" t="n">
         <v>1</v>
@@ -641,16 +659,19 @@
       <c r="M2" s="4" t="n">
         <v>1E-006</v>
       </c>
+      <c r="N2" s="1" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D3" s="4" t="n">
         <v>100000</v>
@@ -662,13 +683,13 @@
         <v>100000</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="J3" s="1" t="n">
         <v>1</v>
@@ -682,16 +703,19 @@
       <c r="M3" s="4" t="n">
         <v>1E-006</v>
       </c>
+      <c r="N3" s="1" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="D4" s="4" t="n">
         <v>100000</v>
@@ -703,13 +727,13 @@
         <v>100000</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="J4" s="1" t="n">
         <v>1</v>
@@ -723,16 +747,19 @@
       <c r="M4" s="4" t="n">
         <v>1E-006</v>
       </c>
+      <c r="N4" s="1" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="D5" s="1" t="n">
         <v>1</v>
@@ -744,13 +771,13 @@
         <v>1</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="J5" s="1" t="n">
         <v>1</v>
@@ -763,6 +790,9 @@
       </c>
       <c r="M5" s="4" t="n">
         <v>1E-006</v>
+      </c>
+      <c r="N5" s="1" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -814,7 +844,7 @@
         <v>5</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="G1" s="5" t="s">
         <v>6</v>
@@ -831,10 +861,10 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C2" s="4" t="n">
         <v>3430000000</v>
@@ -849,10 +879,10 @@
         <v>1</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="I2" s="1" t="str">
         <f aca="false">A2</f>
@@ -865,10 +895,10 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="C3" s="1" t="n">
         <v>0.1</v>
@@ -883,10 +913,10 @@
         <v>1</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="I3" s="1" t="str">
         <f aca="false">A3</f>
@@ -899,10 +929,10 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="C4" s="1" t="n">
         <v>0</v>
@@ -917,10 +947,10 @@
         <v>1</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="I4" s="1" t="str">
         <f aca="false">A4</f>
@@ -933,10 +963,10 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="C5" s="4" t="n">
         <v>5E-006</v>
@@ -951,10 +981,10 @@
         <v>1</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="I5" s="1" t="str">
         <f aca="false">A5</f>
@@ -967,10 +997,10 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="C6" s="4" t="n">
         <v>1.1E-011</v>
@@ -985,24 +1015,24 @@
         <v>1</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="C7" s="4" t="n">
         <v>1.1E-011</v>
@@ -1017,24 +1047,24 @@
         <v>1</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>53</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>48</v>
       </c>
       <c r="C8" s="1" t="n">
         <v>0.22</v>
@@ -1049,10 +1079,10 @@
         <v>0</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="I8" s="1" t="str">
         <f aca="false">A8</f>
@@ -1065,10 +1095,10 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="C9" s="1" t="n">
         <v>0.1</v>
@@ -1083,10 +1113,10 @@
         <v>0</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="I9" s="1" t="str">
         <f aca="false">A9</f>
@@ -1099,10 +1129,10 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="C10" s="1" t="n">
         <v>23.42</v>
@@ -1117,10 +1147,10 @@
         <v>0</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="I10" s="1" t="str">
         <f aca="false">A10</f>
@@ -1133,10 +1163,10 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="C11" s="1" t="n">
         <v>4.52</v>
@@ -1151,10 +1181,10 @@
         <v>0</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="I11" s="1" t="str">
         <f aca="false">A11</f>
@@ -1167,10 +1197,10 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="C12" s="1" t="n">
         <v>0.22</v>
@@ -1185,10 +1215,10 @@
         <v>0</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="I12" s="1" t="str">
         <f aca="false">A12</f>
@@ -1201,10 +1231,10 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="C13" s="1" t="n">
         <v>0.14</v>
@@ -1219,10 +1249,10 @@
         <v>0</v>
       </c>
       <c r="G13" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="H13" s="1" t="s">
         <v>59</v>
-      </c>
-      <c r="H13" s="1" t="s">
-        <v>54</v>
       </c>
       <c r="I13" s="1" t="str">
         <f aca="false">A13</f>
@@ -1235,10 +1265,10 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="C14" s="1" t="n">
         <v>29.6</v>
@@ -1253,10 +1283,10 @@
         <v>0</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="I14" s="1" t="str">
         <f aca="false">A14</f>
@@ -1269,10 +1299,10 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="C15" s="1" t="n">
         <v>0.73</v>
@@ -1287,10 +1317,10 @@
         <v>0</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="I15" s="1" t="str">
         <f aca="false">A15</f>
@@ -1303,10 +1333,10 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="C16" s="1" t="n">
         <v>0.24</v>
@@ -1321,10 +1351,10 @@
         <v>0</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="I16" s="1" t="str">
         <f aca="false">A16</f>
@@ -1337,10 +1367,10 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="C17" s="1" t="n">
         <v>0.08</v>
@@ -1355,10 +1385,10 @@
         <v>0</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="I17" s="1" t="str">
         <f aca="false">A17</f>
@@ -1371,10 +1401,10 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="C18" s="1" t="n">
         <v>25.19</v>
@@ -1389,10 +1419,10 @@
         <v>0</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="I18" s="1" t="str">
         <f aca="false">A18</f>
@@ -1405,10 +1435,10 @@
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="C19" s="1" t="n">
         <v>4.15</v>
@@ -1423,10 +1453,10 @@
         <v>0</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="I19" s="1" t="str">
         <f aca="false">A19</f>
@@ -1439,10 +1469,10 @@
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="C20" s="1" t="n">
         <v>0.5</v>
@@ -1457,10 +1487,10 @@
         <v>0</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="I20" s="1" t="str">
         <f aca="false">A20</f>
@@ -1520,36 +1550,36 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
     </row>
   </sheetData>
@@ -1593,105 +1623,105 @@
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>91</v>
+        <v>96</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
     </row>
   </sheetData>
@@ -1725,145 +1755,145 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>94</v>
+        <v>99</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>95</v>
+        <v>100</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>96</v>
+        <v>101</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>96</v>
+        <v>101</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>99</v>
+        <v>104</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>100</v>
+        <v>105</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>95</v>
+        <v>100</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>96</v>
+        <v>101</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>101</v>
+        <v>106</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>102</v>
+        <v>107</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>96</v>
+        <v>101</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ENH: Optional initialization through steady-state estimation
</commit_message>
<xml_diff>
--- a/inst/examples/DRT/model.xlsx
+++ b/inst/examples/DRT/model.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="120" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="51" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="vars" sheetId="1" state="visible" r:id="rId2"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="109">
   <si>
     <t>name</t>
   </si>
@@ -61,6 +61,9 @@
   </si>
   <si>
     <t>color</t>
+  </si>
+  <si>
+    <t>steady</t>
   </si>
   <si>
     <t>A</t>
@@ -562,10 +565,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:N5"/>
+  <dimension ref="A1:O5"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N6" activeCellId="0" sqref="N6"/>
+      <selection pane="topLeft" activeCell="O6" activeCellId="0" sqref="O6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -618,16 +621,19 @@
       <c r="N1" s="3" t="s">
         <v>13</v>
       </c>
+      <c r="O1" s="2" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D2" s="1" t="n">
         <v>0</v>
@@ -639,13 +645,13 @@
         <v>2.5</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="J2" s="1" t="n">
         <v>1</v>
@@ -660,18 +666,21 @@
         <v>1E-006</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
+      </c>
+      <c r="O2" s="1" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D3" s="4" t="n">
         <v>100000</v>
@@ -683,13 +692,13 @@
         <v>100000</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="J3" s="1" t="n">
         <v>1</v>
@@ -704,18 +713,21 @@
         <v>1E-006</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
+      </c>
+      <c r="O3" s="1" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D4" s="4" t="n">
         <v>100000</v>
@@ -727,13 +739,13 @@
         <v>100000</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="J4" s="1" t="n">
         <v>1</v>
@@ -748,36 +760,39 @@
         <v>1E-006</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
+      </c>
+      <c r="O4" s="1" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C5" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D5" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E5" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="F5" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="H5" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D5" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="E5" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="F5" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>28</v>
-      </c>
       <c r="I5" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="J5" s="1" t="n">
         <v>1</v>
@@ -792,7 +807,10 @@
         <v>1E-006</v>
       </c>
       <c r="N5" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
+      </c>
+      <c r="O5" s="1" t="n">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -844,7 +862,7 @@
         <v>5</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G1" s="5" t="s">
         <v>6</v>
@@ -861,10 +879,10 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C2" s="4" t="n">
         <v>3430000000</v>
@@ -879,10 +897,10 @@
         <v>1</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="I2" s="1" t="str">
         <f aca="false">A2</f>
@@ -895,10 +913,10 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C3" s="1" t="n">
         <v>0.1</v>
@@ -913,10 +931,10 @@
         <v>1</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="I3" s="1" t="str">
         <f aca="false">A3</f>
@@ -929,10 +947,10 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C4" s="1" t="n">
         <v>0</v>
@@ -947,10 +965,10 @@
         <v>1</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="I4" s="1" t="str">
         <f aca="false">A4</f>
@@ -963,10 +981,10 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C5" s="4" t="n">
         <v>5E-006</v>
@@ -981,10 +999,10 @@
         <v>1</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="I5" s="1" t="str">
         <f aca="false">A5</f>
@@ -997,10 +1015,10 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C6" s="4" t="n">
         <v>1.1E-011</v>
@@ -1015,24 +1033,24 @@
         <v>1</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C7" s="4" t="n">
         <v>1.1E-011</v>
@@ -1047,24 +1065,24 @@
         <v>1</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C8" s="1" t="n">
         <v>0.22</v>
@@ -1079,10 +1097,10 @@
         <v>0</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="I8" s="1" t="str">
         <f aca="false">A8</f>
@@ -1095,10 +1113,10 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C9" s="1" t="n">
         <v>0.1</v>
@@ -1113,10 +1131,10 @@
         <v>0</v>
       </c>
       <c r="G9" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="H9" s="1" t="s">
         <v>60</v>
-      </c>
-      <c r="H9" s="1" t="s">
-        <v>59</v>
       </c>
       <c r="I9" s="1" t="str">
         <f aca="false">A9</f>
@@ -1129,10 +1147,10 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C10" s="1" t="n">
         <v>23.42</v>
@@ -1147,10 +1165,10 @@
         <v>0</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="I10" s="1" t="str">
         <f aca="false">A10</f>
@@ -1163,10 +1181,10 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C11" s="1" t="n">
         <v>4.52</v>
@@ -1181,10 +1199,10 @@
         <v>0</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="I11" s="1" t="str">
         <f aca="false">A11</f>
@@ -1197,10 +1215,10 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C12" s="1" t="n">
         <v>0.22</v>
@@ -1215,10 +1233,10 @@
         <v>0</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="I12" s="1" t="str">
         <f aca="false">A12</f>
@@ -1231,10 +1249,10 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C13" s="1" t="n">
         <v>0.14</v>
@@ -1249,10 +1267,10 @@
         <v>0</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="I13" s="1" t="str">
         <f aca="false">A13</f>
@@ -1265,10 +1283,10 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C14" s="1" t="n">
         <v>29.6</v>
@@ -1283,10 +1301,10 @@
         <v>0</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="I14" s="1" t="str">
         <f aca="false">A14</f>
@@ -1299,10 +1317,10 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C15" s="1" t="n">
         <v>0.73</v>
@@ -1317,10 +1335,10 @@
         <v>0</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="I15" s="1" t="str">
         <f aca="false">A15</f>
@@ -1333,10 +1351,10 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C16" s="1" t="n">
         <v>0.24</v>
@@ -1351,10 +1369,10 @@
         <v>0</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="I16" s="1" t="str">
         <f aca="false">A16</f>
@@ -1367,10 +1385,10 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C17" s="1" t="n">
         <v>0.08</v>
@@ -1385,10 +1403,10 @@
         <v>0</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="I17" s="1" t="str">
         <f aca="false">A17</f>
@@ -1401,10 +1419,10 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C18" s="1" t="n">
         <v>25.19</v>
@@ -1419,10 +1437,10 @@
         <v>0</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="I18" s="1" t="str">
         <f aca="false">A18</f>
@@ -1435,10 +1453,10 @@
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C19" s="1" t="n">
         <v>4.15</v>
@@ -1453,10 +1471,10 @@
         <v>0</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="I19" s="1" t="str">
         <f aca="false">A19</f>
@@ -1469,10 +1487,10 @@
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C20" s="1" t="n">
         <v>0.5</v>
@@ -1487,10 +1505,10 @@
         <v>0</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="I20" s="1" t="str">
         <f aca="false">A20</f>
@@ -1550,36 +1568,36 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>72</v>
-      </c>
       <c r="E2" s="1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>74</v>
-      </c>
       <c r="E3" s="1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
   </sheetData>
@@ -1623,105 +1641,105 @@
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>37</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
   </sheetData>
@@ -1755,145 +1773,145 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
MIN: Disabled test of steady-state initialization in example model
</commit_message>
<xml_diff>
--- a/inst/examples/DRT/model.xlsx
+++ b/inst/examples/DRT/model.xlsx
@@ -716,7 +716,7 @@
         <v>24</v>
       </c>
       <c r="O3" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -763,7 +763,7 @@
         <v>28</v>
       </c>
       <c r="O4" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -810,7 +810,7 @@
         <v>32</v>
       </c>
       <c r="O5" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ENH: Updated functional response in bacteria example model
</commit_message>
<xml_diff>
--- a/inst/examples/DRT/model.xlsx
+++ b/inst/examples/DRT/model.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="51" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="432" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="vars" sheetId="1" state="visible" r:id="rId2"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="126">
   <si>
     <t>name</t>
   </si>
@@ -198,58 +198,109 @@
     <t>mult&lt;sub&gt;TR&lt;/sub&gt;</t>
   </si>
   <si>
-    <t>aD</t>
-  </si>
-  <si>
-    <t>empirical par.</t>
-  </si>
-  <si>
-    <t>bD</t>
-  </si>
-  <si>
-    <t>pD</t>
-  </si>
-  <si>
-    <t>qD</t>
-  </si>
-  <si>
-    <t>aR</t>
-  </si>
-  <si>
-    <t>bR</t>
-  </si>
-  <si>
-    <t>pR</t>
-  </si>
-  <si>
-    <t>qR</t>
-  </si>
-  <si>
-    <t>aT</t>
-  </si>
-  <si>
-    <t>bT</t>
-  </si>
-  <si>
-    <t>pT</t>
-  </si>
-  <si>
-    <t>qT</t>
-  </si>
-  <si>
-    <t>z</t>
-  </si>
-  <si>
-    <t>fun</t>
-  </si>
-  <si>
-    <t>growth rate under possible antibiotic treatment</t>
+    <t>muD</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>mu max. (D)</t>
+  </si>
+  <si>
+    <t>max. growth rate of D</t>
+  </si>
+  <si>
+    <t>\mu_D</t>
+  </si>
+  <si>
+    <t>mu&lt;sub&gt;D&lt;/sub&gt;</t>
+  </si>
+  <si>
+    <t>muT</t>
+  </si>
+  <si>
+    <t>mu max. (T)</t>
+  </si>
+  <si>
+    <t>max. growth rate of T</t>
+  </si>
+  <si>
+    <t>\mu_T</t>
+  </si>
+  <si>
+    <t>mu&lt;sub&gt;T&lt;/sub&gt;</t>
+  </si>
+  <si>
+    <t>muR</t>
+  </si>
+  <si>
+    <t>mu max. (R)</t>
+  </si>
+  <si>
+    <t>max. growth rate of R</t>
+  </si>
+  <si>
+    <t>\mu_R</t>
+  </si>
+  <si>
+    <t>mu&lt;sub&gt;R&lt;/sub&gt;</t>
+  </si>
+  <si>
+    <t>micD</t>
+  </si>
+  <si>
+    <t>MIC (D)</t>
+  </si>
+  <si>
+    <t>MIC for D</t>
+  </si>
+  <si>
+    <t>MIC_D</t>
+  </si>
+  <si>
+    <t>MIC&lt;sub&gt;D&lt;/sub&gt;</t>
+  </si>
+  <si>
+    <t>micT</t>
+  </si>
+  <si>
+    <t>MIC (T)</t>
+  </si>
+  <si>
+    <t>MIC for T</t>
+  </si>
+  <si>
+    <t>MIC_T</t>
+  </si>
+  <si>
+    <t>MIC&lt;sub&gt;T&lt;/sub&gt;</t>
+  </si>
+  <si>
+    <t>micR</t>
+  </si>
+  <si>
+    <t>MIC (R)</t>
+  </si>
+  <si>
+    <t>MIC for R</t>
+  </si>
+  <si>
+    <t>MIC_R</t>
+  </si>
+  <si>
+    <t>MIC&lt;sub&gt;R&lt;/sub&gt;</t>
+  </si>
+  <si>
+    <t>fa</t>
+  </si>
+  <si>
+    <t>growth inhibition term (range 0 ... 1)</t>
   </si>
   <si>
     <t>fk</t>
   </si>
   <si>
-    <t>ressource limitation term</t>
+    <t>ressource limitation term (range 0 ... 1)</t>
   </si>
   <si>
     <t>expression</t>
@@ -264,7 +315,7 @@
     <t>growth of donor</t>
   </si>
   <si>
-    <t>fk(K,D,R,T) * fun(A,z,aD,bD,pD,qD) * D</t>
+    <t>muD * fk(K,D,R,T) * fa(A,micD) * D</t>
   </si>
   <si>
     <t>growthR</t>
@@ -273,7 +324,7 @@
     <t>growth of recipient</t>
   </si>
   <si>
-    <t>fk(K,D,R,T) * fun(A,z,aR,bR,pR,qR) * R</t>
+    <t>muR * fk(K,D,R,T) * fa(A,micR) * R</t>
   </si>
   <si>
     <t>growthT</t>
@@ -282,7 +333,7 @@
     <t>growth of transconjugant</t>
   </si>
   <si>
-    <t>fk(K,D,R,T) * fun(A,z,aT,bT,pT,qT) * T</t>
+    <t>muT * fk(K,D,R,T) * fa(A,micT) * T</t>
   </si>
   <si>
     <t>predation</t>
@@ -333,19 +384,19 @@
     <t>-D</t>
   </si>
   <si>
-    <t>-fun(A,z,aD,bD,pD,qD) * D</t>
+    <t>- muD * fa(A,micD) * D</t>
   </si>
   <si>
     <t>-R</t>
   </si>
   <si>
-    <t>fun(A,z,aD,bD,pD,qD) * D + fun(A,z,aT,bT,pT,qT) * T</t>
+    <t>muD * fa(A,micD) * D + muT * fa(A,micT) * T</t>
   </si>
   <si>
     <t>-T</t>
   </si>
   <si>
-    <t>-fun(A,z,aT,bT,pT,qT) * T</t>
+    <t>- muT * fa(A,micT) * T</t>
   </si>
 </sst>
 </file>
@@ -455,7 +506,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -477,6 +528,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -567,7 +622,7 @@
   </sheetPr>
   <dimension ref="A1:O5"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="O6" activeCellId="0" sqref="O6"/>
     </sheetView>
   </sheetViews>
@@ -829,10 +884,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J20"/>
+  <dimension ref="A1:J13"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I1" activeCellId="0" sqref="I1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1053,7 +1108,7 @@
         <v>54</v>
       </c>
       <c r="C7" s="4" t="n">
-        <v>1.1E-011</v>
+        <v>1</v>
       </c>
       <c r="D7" s="4" t="n">
         <v>5.5E-012</v>
@@ -1078,445 +1133,195 @@
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1" t="s">
+      <c r="A8" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="C8" s="1" t="n">
-        <v>0.22</v>
-      </c>
-      <c r="D8" s="1" t="n">
-        <v>0.22</v>
-      </c>
-      <c r="E8" s="1" t="n">
-        <v>0.22</v>
-      </c>
-      <c r="F8" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="H8" s="1" t="s">
+      <c r="B8" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C8" s="6" t="n">
+        <v>0.894</v>
+      </c>
+      <c r="D8" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="I8" s="1" t="str">
-        <f aca="false">A8</f>
-        <v>aD</v>
-      </c>
-      <c r="J8" s="1" t="str">
-        <f aca="false">A8</f>
-        <v>aD</v>
+      <c r="E8" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="F8" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="G8" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="H8" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="I8" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="C9" s="1" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="D9" s="1" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="E9" s="1" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="F9" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="H9" s="1" t="s">
+      <c r="A9" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C9" s="6" t="n">
+        <v>0.906</v>
+      </c>
+      <c r="D9" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="I9" s="1" t="str">
-        <f aca="false">A9</f>
-        <v>bD</v>
-      </c>
-      <c r="J9" s="1" t="str">
-        <f aca="false">A9</f>
-        <v>bD</v>
+      <c r="E9" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="F9" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="G9" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="H9" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="I9" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="C10" s="1" t="n">
-        <v>23.42</v>
-      </c>
-      <c r="D10" s="1" t="n">
-        <v>23.42</v>
-      </c>
-      <c r="E10" s="1" t="n">
-        <v>23.42</v>
-      </c>
-      <c r="F10" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="H10" s="1" t="s">
+      <c r="A10" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C10" s="6" t="n">
+        <v>0.938</v>
+      </c>
+      <c r="D10" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="I10" s="1" t="str">
-        <f aca="false">A10</f>
-        <v>pD</v>
-      </c>
-      <c r="J10" s="1" t="str">
-        <f aca="false">A10</f>
-        <v>pD</v>
+      <c r="E10" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="F10" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="G10" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="H10" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="I10" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>63</v>
+        <v>75</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="C11" s="1" t="n">
-        <v>4.52</v>
-      </c>
-      <c r="D11" s="1" t="n">
-        <v>4.52</v>
-      </c>
-      <c r="E11" s="1" t="n">
-        <v>4.52</v>
+        <v>16</v>
+      </c>
+      <c r="C11" s="4" t="n">
+        <v>50</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>60</v>
       </c>
       <c r="F11" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>63</v>
+        <v>76</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="I11" s="1" t="str">
-        <f aca="false">A11</f>
-        <v>qD</v>
-      </c>
-      <c r="J11" s="1" t="str">
-        <f aca="false">A11</f>
-        <v>qD</v>
+        <v>77</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>64</v>
+        <v>80</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="C12" s="1" t="n">
-        <v>0.22</v>
-      </c>
-      <c r="D12" s="1" t="n">
-        <v>0.22</v>
-      </c>
-      <c r="E12" s="1" t="n">
-        <v>0.22</v>
+        <v>16</v>
+      </c>
+      <c r="C12" s="4" t="n">
+        <v>50</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>60</v>
       </c>
       <c r="F12" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>64</v>
+        <v>81</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="I12" s="1" t="str">
-        <f aca="false">A12</f>
-        <v>aR</v>
-      </c>
-      <c r="J12" s="1" t="str">
-        <f aca="false">A12</f>
-        <v>aR</v>
+        <v>82</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="J12" s="1" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>65</v>
+        <v>85</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>54</v>
+        <v>16</v>
       </c>
       <c r="C13" s="1" t="n">
-        <v>0.14</v>
-      </c>
-      <c r="D13" s="1" t="n">
-        <v>0.14</v>
-      </c>
-      <c r="E13" s="1" t="n">
-        <v>0.14</v>
+        <v>0.3</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>60</v>
       </c>
       <c r="F13" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>65</v>
+        <v>86</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="I13" s="1" t="str">
-        <f aca="false">A13</f>
-        <v>bR</v>
-      </c>
-      <c r="J13" s="1" t="str">
-        <f aca="false">A13</f>
-        <v>bR</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="C14" s="1" t="n">
-        <v>29.6</v>
-      </c>
-      <c r="D14" s="1" t="n">
-        <v>29.6</v>
-      </c>
-      <c r="E14" s="1" t="n">
-        <v>29.6</v>
-      </c>
-      <c r="F14" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="G14" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="H14" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="I14" s="1" t="str">
-        <f aca="false">A14</f>
-        <v>pR</v>
-      </c>
-      <c r="J14" s="1" t="str">
-        <f aca="false">A14</f>
-        <v>pR</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="C15" s="1" t="n">
-        <v>0.73</v>
-      </c>
-      <c r="D15" s="1" t="n">
-        <v>0.73</v>
-      </c>
-      <c r="E15" s="1" t="n">
-        <v>0.73</v>
-      </c>
-      <c r="F15" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="G15" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="H15" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="I15" s="1" t="str">
-        <f aca="false">A15</f>
-        <v>qR</v>
-      </c>
-      <c r="J15" s="1" t="str">
-        <f aca="false">A15</f>
-        <v>qR</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="C16" s="1" t="n">
-        <v>0.24</v>
-      </c>
-      <c r="D16" s="1" t="n">
-        <v>0.24</v>
-      </c>
-      <c r="E16" s="1" t="n">
-        <v>0.24</v>
-      </c>
-      <c r="F16" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="G16" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="H16" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="I16" s="1" t="str">
-        <f aca="false">A16</f>
-        <v>aT</v>
-      </c>
-      <c r="J16" s="1" t="str">
-        <f aca="false">A16</f>
-        <v>aT</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="C17" s="1" t="n">
-        <v>0.08</v>
-      </c>
-      <c r="D17" s="1" t="n">
-        <v>0.08</v>
-      </c>
-      <c r="E17" s="1" t="n">
-        <v>0.08</v>
-      </c>
-      <c r="F17" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="G17" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="H17" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="I17" s="1" t="str">
-        <f aca="false">A17</f>
-        <v>bT</v>
-      </c>
-      <c r="J17" s="1" t="str">
-        <f aca="false">A17</f>
-        <v>bT</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="C18" s="1" t="n">
-        <v>25.19</v>
-      </c>
-      <c r="D18" s="1" t="n">
-        <v>25.19</v>
-      </c>
-      <c r="E18" s="1" t="n">
-        <v>25.19</v>
-      </c>
-      <c r="F18" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="G18" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="H18" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="I18" s="1" t="str">
-        <f aca="false">A18</f>
-        <v>pT</v>
-      </c>
-      <c r="J18" s="1" t="str">
-        <f aca="false">A18</f>
-        <v>pT</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="C19" s="1" t="n">
-        <v>4.15</v>
-      </c>
-      <c r="D19" s="1" t="n">
-        <v>4.15</v>
-      </c>
-      <c r="E19" s="1" t="n">
-        <v>4.15</v>
-      </c>
-      <c r="F19" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="G19" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="H19" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="I19" s="1" t="str">
-        <f aca="false">A19</f>
-        <v>qT</v>
-      </c>
-      <c r="J19" s="1" t="str">
-        <f aca="false">A19</f>
-        <v>qT</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="C20" s="1" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="D20" s="1" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="E20" s="1" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="F20" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="G20" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="H20" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="I20" s="1" t="str">
-        <f aca="false">A20</f>
-        <v>z</v>
-      </c>
-      <c r="J20" s="1" t="str">
-        <f aca="false">A20</f>
-        <v>z</v>
+        <v>87</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>89</v>
       </c>
     </row>
   </sheetData>
@@ -1538,7 +1343,7 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E4" activeCellId="0" sqref="E4"/>
+      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1568,36 +1373,36 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>73</v>
+        <v>90</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>54</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>74</v>
+        <v>91</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>73</v>
+        <v>90</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>73</v>
+        <v>90</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>75</v>
+        <v>92</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>54</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>76</v>
+        <v>93</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>75</v>
+        <v>92</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>75</v>
+        <v>92</v>
       </c>
     </row>
   </sheetData>
@@ -1619,7 +1424,7 @@
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
+      <selection pane="topLeft" activeCell="D9" activeCellId="0" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1641,60 +1446,60 @@
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>77</v>
+        <v>94</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>78</v>
+        <v>95</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>79</v>
+        <v>96</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>80</v>
+        <v>97</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>81</v>
+        <v>98</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>82</v>
+        <v>99</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>79</v>
+        <v>96</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>83</v>
+        <v>100</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>84</v>
+        <v>101</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>85</v>
+        <v>102</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>79</v>
+        <v>96</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>86</v>
+        <v>103</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>87</v>
+        <v>104</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>88</v>
+        <v>105</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>38</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>89</v>
+        <v>106</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>37</v>
@@ -1702,44 +1507,44 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>90</v>
+        <v>107</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>79</v>
+        <v>96</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>91</v>
+        <v>108</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>92</v>
+        <v>109</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>93</v>
+        <v>110</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>38</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>94</v>
+        <v>111</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>95</v>
+        <v>112</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>96</v>
+        <v>113</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>38</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>97</v>
+        <v>114</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>98</v>
+        <v>115</v>
       </c>
     </row>
   </sheetData>
@@ -1761,7 +1566,7 @@
   <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C26" activeCellId="0" sqref="C26"/>
+      <selection pane="topLeft" activeCell="C13" activeCellId="0" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1773,13 +1578,13 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>99</v>
+        <v>116</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="C1" s="6" t="s">
-        <v>77</v>
+        <v>117</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1787,10 +1592,10 @@
         <v>15</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>101</v>
+        <v>113</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1798,10 +1603,10 @@
         <v>20</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="C3" s="7" t="s">
-        <v>102</v>
+        <v>95</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1809,10 +1614,10 @@
         <v>20</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>103</v>
+        <v>105</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1820,10 +1625,10 @@
         <v>20</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="C5" s="7" t="s">
-        <v>104</v>
+        <v>110</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1831,10 +1636,10 @@
         <v>25</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>102</v>
+        <v>99</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1842,10 +1647,10 @@
         <v>25</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="C7" s="7" t="s">
         <v>105</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1853,10 +1658,10 @@
         <v>25</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="C8" s="7" t="s">
-        <v>106</v>
+        <v>110</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1864,10 +1669,10 @@
         <v>25</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="C9" s="7" t="s">
-        <v>101</v>
+        <v>107</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1875,10 +1680,10 @@
         <v>29</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="C10" s="7" t="s">
         <v>102</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1886,10 +1691,10 @@
         <v>29</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="C11" s="7" t="s">
-        <v>107</v>
+        <v>105</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1897,10 +1702,10 @@
         <v>29</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="C12" s="7" t="s">
-        <v>108</v>
+        <v>110</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1908,10 +1713,10 @@
         <v>29</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="C13" s="7" t="s">
-        <v>102</v>
+        <v>107</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>119</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ENH: Updated DRT example model
</commit_message>
<xml_diff>
--- a/inst/examples/DRT/model.xlsx
+++ b/inst/examples/DRT/model.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="432" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="298" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="vars" sheetId="1" state="visible" r:id="rId2"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="162">
   <si>
     <t>name</t>
   </si>
@@ -291,18 +291,123 @@
     <t>MIC&lt;sub&gt;R&lt;/sub&gt;</t>
   </si>
   <si>
-    <t>fa</t>
+    <t>c50D</t>
+  </si>
+  <si>
+    <t>c50 (D)</t>
+  </si>
+  <si>
+    <t>inflection point of functional response, for D</t>
+  </si>
+  <si>
+    <t>c50_D</t>
+  </si>
+  <si>
+    <t>c50&lt;sub&gt;D&lt;/sub&gt;</t>
+  </si>
+  <si>
+    <t>c50T</t>
+  </si>
+  <si>
+    <t>c50 (T)</t>
+  </si>
+  <si>
+    <t>inflection point of functional response, for T</t>
+  </si>
+  <si>
+    <t>c50_T</t>
+  </si>
+  <si>
+    <t>c50&lt;sub&gt;T&lt;/sub&gt;</t>
+  </si>
+  <si>
+    <t>c50R</t>
+  </si>
+  <si>
+    <t>c50 (R)</t>
+  </si>
+  <si>
+    <t>inflection point of functional response, for R</t>
+  </si>
+  <si>
+    <t>c50_R</t>
+  </si>
+  <si>
+    <t>c50&lt;sub&gt;R&lt;/sub&gt;</t>
+  </si>
+  <si>
+    <t>slpD</t>
+  </si>
+  <si>
+    <t>L/mg</t>
+  </si>
+  <si>
+    <t>slp (D)</t>
+  </si>
+  <si>
+    <t>slope of tangent of functional response, for D</t>
+  </si>
+  <si>
+    <t>slp_D</t>
+  </si>
+  <si>
+    <t>slp&lt;sub&gt;D&lt;/sub&gt;</t>
+  </si>
+  <si>
+    <t>slpT</t>
+  </si>
+  <si>
+    <t>slp (T)</t>
+  </si>
+  <si>
+    <t>slope of tangent of functional response, for T</t>
+  </si>
+  <si>
+    <t>slp_T</t>
+  </si>
+  <si>
+    <t>slp&lt;sub&gt;T&lt;/sub&gt;</t>
+  </si>
+  <si>
+    <t>slpR</t>
+  </si>
+  <si>
+    <t>slp (R)</t>
+  </si>
+  <si>
+    <t>slope of tangent of functional response, for R</t>
+  </si>
+  <si>
+    <t>slp_R</t>
+  </si>
+  <si>
+    <t>slp&lt;sub&gt;R&lt;/sub&gt;</t>
+  </si>
+  <si>
+    <t>use_mic</t>
+  </si>
+  <si>
+    <t>use MIC?</t>
+  </si>
+  <si>
+    <t>Either 1 or 0; switch to select functional response</t>
+  </si>
+  <si>
+    <t>useMIC</t>
+  </si>
+  <si>
+    <t>fk</t>
+  </si>
+  <si>
+    <t>ressource limitation term (range 0 ... 1)</t>
+  </si>
+  <si>
+    <t>rsp</t>
   </si>
   <si>
     <t>growth inhibition term (range 0 ... 1)</t>
   </si>
   <si>
-    <t>fk</t>
-  </si>
-  <si>
-    <t>ressource limitation term (range 0 ... 1)</t>
-  </si>
-  <si>
     <t>expression</t>
   </si>
   <si>
@@ -315,7 +420,7 @@
     <t>growth of donor</t>
   </si>
   <si>
-    <t>muD * fk(K,D,R,T) * fa(A,micD) * D</t>
+    <t>muD * fk(K,D,R,T) * rsp(A,micD,use_mic,c50D,slpD) * D</t>
   </si>
   <si>
     <t>growthR</t>
@@ -324,7 +429,7 @@
     <t>growth of recipient</t>
   </si>
   <si>
-    <t>muR * fk(K,D,R,T) * fa(A,micR) * R</t>
+    <t>muR * fk(K,D,R,T) * rsp(A,micR,use_mic,c50R,slpR) * R</t>
   </si>
   <si>
     <t>growthT</t>
@@ -333,7 +438,7 @@
     <t>growth of transconjugant</t>
   </si>
   <si>
-    <t>muT * fk(K,D,R,T) * fa(A,micT) * T</t>
+    <t>muT * fk(K,D,R,T) * rsp(A,micT,use_mic,c50T,slpT) * T</t>
   </si>
   <si>
     <t>predation</t>
@@ -363,6 +468,9 @@
     <t>decay</t>
   </si>
   <si>
+    <t>mg/L/h</t>
+  </si>
+  <si>
     <t>decay of antibiotic</t>
   </si>
   <si>
@@ -384,19 +492,19 @@
     <t>-D</t>
   </si>
   <si>
-    <t>- muD * fa(A,micD) * D</t>
+    <t>- muD * rsp(A,micD,use_mic,c50D,slpD) * D</t>
   </si>
   <si>
     <t>-R</t>
   </si>
   <si>
-    <t>muD * fa(A,micD) * D + muT * fa(A,micT) * T</t>
+    <t>muD * rsp(A,micD,use_mic,c50D,slpD) * D + muT * rsp(A,micT,use_mic,c50T,slpT) * T</t>
   </si>
   <si>
     <t>-T</t>
   </si>
   <si>
-    <t>- muT * fa(A,micT) * T</t>
+    <t>- muT * rsp(A,micT,use_mic,c50T,slpT) * T</t>
   </si>
 </sst>
 </file>
@@ -623,7 +731,7 @@
   <dimension ref="A1:O5"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="O6" activeCellId="0" sqref="O6"/>
+      <selection pane="topLeft" activeCell="C26" activeCellId="0" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -884,10 +992,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J13"/>
+  <dimension ref="A1:J20"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D10" activeCellId="0" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -942,11 +1050,13 @@
       <c r="C2" s="4" t="n">
         <v>3430000000</v>
       </c>
-      <c r="D2" s="4" t="n">
-        <v>1720000000</v>
-      </c>
-      <c r="E2" s="4" t="n">
-        <v>6860000000</v>
+      <c r="D2" s="6" t="n">
+        <f aca="false">C2*0.8</f>
+        <v>2744000000</v>
+      </c>
+      <c r="E2" s="6" t="n">
+        <f aca="false">C2*1.2</f>
+        <v>4116000000</v>
       </c>
       <c r="F2" s="1" t="n">
         <v>1</v>
@@ -976,11 +1086,13 @@
       <c r="C3" s="1" t="n">
         <v>0.1</v>
       </c>
-      <c r="D3" s="4" t="n">
-        <v>0.05</v>
-      </c>
-      <c r="E3" s="4" t="n">
-        <v>0.2</v>
+      <c r="D3" s="6" t="n">
+        <f aca="false">C3*0.8</f>
+        <v>0.08</v>
+      </c>
+      <c r="E3" s="6" t="n">
+        <f aca="false">C3*1.2</f>
+        <v>0.12</v>
       </c>
       <c r="F3" s="1" t="n">
         <v>1</v>
@@ -1010,10 +1122,12 @@
       <c r="C4" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="D4" s="4" t="n">
+      <c r="D4" s="6" t="n">
+        <f aca="false">C4*0.8</f>
         <v>0</v>
       </c>
-      <c r="E4" s="4" t="n">
+      <c r="E4" s="6" t="n">
+        <f aca="false">C4*1.2</f>
         <v>0</v>
       </c>
       <c r="F4" s="1" t="n">
@@ -1044,11 +1158,13 @@
       <c r="C5" s="4" t="n">
         <v>5E-006</v>
       </c>
-      <c r="D5" s="4" t="n">
-        <v>2.5E-006</v>
-      </c>
-      <c r="E5" s="4" t="n">
-        <v>1E-005</v>
+      <c r="D5" s="6" t="n">
+        <f aca="false">C5*0.8</f>
+        <v>4E-006</v>
+      </c>
+      <c r="E5" s="6" t="n">
+        <f aca="false">C5*1.2</f>
+        <v>6E-006</v>
       </c>
       <c r="F5" s="1" t="n">
         <v>1</v>
@@ -1078,11 +1194,13 @@
       <c r="C6" s="4" t="n">
         <v>1.1E-011</v>
       </c>
-      <c r="D6" s="4" t="n">
-        <v>5.5E-012</v>
-      </c>
-      <c r="E6" s="4" t="n">
-        <v>2.2E-011</v>
+      <c r="D6" s="6" t="n">
+        <f aca="false">C6*0.8</f>
+        <v>8.8E-012</v>
+      </c>
+      <c r="E6" s="6" t="n">
+        <f aca="false">C6*1.2</f>
+        <v>1.32E-011</v>
       </c>
       <c r="F6" s="1" t="n">
         <v>1</v>
@@ -1110,11 +1228,13 @@
       <c r="C7" s="4" t="n">
         <v>1</v>
       </c>
-      <c r="D7" s="4" t="n">
-        <v>5.5E-012</v>
-      </c>
-      <c r="E7" s="4" t="n">
-        <v>2.2E-011</v>
+      <c r="D7" s="6" t="n">
+        <f aca="false">C7*0.8</f>
+        <v>0.8</v>
+      </c>
+      <c r="E7" s="6" t="n">
+        <f aca="false">C7*1.2</f>
+        <v>1.2</v>
       </c>
       <c r="F7" s="1" t="n">
         <v>1</v>
@@ -1236,7 +1356,7 @@
         <v>16</v>
       </c>
       <c r="C11" s="4" t="n">
-        <v>50</v>
+        <v>33.8</v>
       </c>
       <c r="D11" s="6" t="s">
         <v>60</v>
@@ -1268,7 +1388,7 @@
         <v>16</v>
       </c>
       <c r="C12" s="4" t="n">
-        <v>50</v>
+        <v>28.5</v>
       </c>
       <c r="D12" s="6" t="s">
         <v>60</v>
@@ -1300,7 +1420,7 @@
         <v>16</v>
       </c>
       <c r="C13" s="1" t="n">
-        <v>0.3</v>
+        <v>0.396</v>
       </c>
       <c r="D13" s="6" t="s">
         <v>60</v>
@@ -1322,6 +1442,230 @@
       </c>
       <c r="J13" s="1" t="s">
         <v>89</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C14" s="4" t="n">
+        <v>16.7</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="F14" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="J14" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C15" s="4" t="n">
+        <v>11.2</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="E15" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="F15" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="J15" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C16" s="1" t="n">
+        <v>0.186</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="E16" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="F16" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="J16" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="C17" s="4" t="n">
+        <v>0.296</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="E17" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="F17" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="J17" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="C18" s="4" t="n">
+        <v>0.147</v>
+      </c>
+      <c r="D18" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="E18" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="F18" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="J18" s="1" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="C19" s="1" t="n">
+        <v>13.2</v>
+      </c>
+      <c r="D19" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="E19" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="F19" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="I19" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="J19" s="1" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C20" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D20" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="E20" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="F20" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="I20" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="J20" s="1" t="s">
+        <v>124</v>
       </c>
     </row>
   </sheetData>
@@ -1343,13 +1687,13 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
+      <selection pane="topLeft" activeCell="C21" activeCellId="0" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="2" min="1" style="1" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="47.5867346938776"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="53.2295918367347"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="1" width="6.44387755102041"/>
     <col collapsed="false" hidden="false" max="1025" min="5" style="1" width="11.5204081632653"/>
   </cols>
@@ -1373,36 +1717,36 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>90</v>
+        <v>125</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>54</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>91</v>
+        <v>126</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>90</v>
+        <v>125</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>90</v>
+        <v>125</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>92</v>
+        <v>127</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>54</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>93</v>
+        <v>128</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>92</v>
+        <v>127</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>92</v>
+        <v>127</v>
       </c>
     </row>
   </sheetData>
@@ -1423,8 +1767,8 @@
   </sheetPr>
   <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D9" activeCellId="0" sqref="D9"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1446,60 +1790,60 @@
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>94</v>
+        <v>129</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>95</v>
+        <v>130</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>96</v>
+        <v>131</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>97</v>
+        <v>132</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>98</v>
+        <v>133</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>99</v>
+        <v>134</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>96</v>
+        <v>131</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>100</v>
+        <v>135</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>101</v>
+        <v>136</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>102</v>
+        <v>137</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>96</v>
+        <v>131</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>103</v>
+        <v>138</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>104</v>
+        <v>139</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>105</v>
+        <v>140</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>38</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>106</v>
+        <v>141</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>37</v>
@@ -1507,44 +1851,44 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>107</v>
+        <v>142</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>96</v>
+        <v>131</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>108</v>
+        <v>143</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>109</v>
+        <v>144</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>110</v>
+        <v>145</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>38</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>111</v>
+        <v>146</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>112</v>
+        <v>147</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>113</v>
+        <v>148</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>38</v>
+        <v>149</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>114</v>
+        <v>150</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>115</v>
+        <v>151</v>
       </c>
     </row>
   </sheetData>
@@ -1566,7 +1910,7 @@
   <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C13" activeCellId="0" sqref="C13"/>
+      <selection pane="topLeft" activeCell="C15" activeCellId="0" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1578,13 +1922,13 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>116</v>
+        <v>152</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>117</v>
+        <v>153</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>94</v>
+        <v>129</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1592,10 +1936,10 @@
         <v>15</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>113</v>
+        <v>148</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>118</v>
+        <v>154</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1603,10 +1947,10 @@
         <v>20</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>95</v>
+        <v>130</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>119</v>
+        <v>155</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1614,10 +1958,10 @@
         <v>20</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>105</v>
+        <v>140</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>120</v>
+        <v>156</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1625,10 +1969,10 @@
         <v>20</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>110</v>
+        <v>145</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>121</v>
+        <v>157</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1636,10 +1980,10 @@
         <v>25</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>99</v>
+        <v>134</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>119</v>
+        <v>155</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1647,10 +1991,10 @@
         <v>25</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>105</v>
+        <v>140</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>122</v>
+        <v>158</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1658,10 +2002,10 @@
         <v>25</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>110</v>
+        <v>145</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>123</v>
+        <v>159</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1669,10 +2013,10 @@
         <v>25</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>107</v>
+        <v>142</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>118</v>
+        <v>154</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1680,10 +2024,10 @@
         <v>29</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>102</v>
+        <v>137</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>119</v>
+        <v>155</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1691,10 +2035,10 @@
         <v>29</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>105</v>
+        <v>140</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>124</v>
+        <v>160</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1702,10 +2046,10 @@
         <v>29</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>110</v>
+        <v>145</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>125</v>
+        <v>161</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1713,10 +2057,10 @@
         <v>29</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>107</v>
+        <v>142</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>119</v>
+        <v>155</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
MIN: Changed default values of parameters in DRT example
</commit_message>
<xml_diff>
--- a/inst/examples/DRT/model.xlsx
+++ b/inst/examples/DRT/model.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="298" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="298" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="vars" sheetId="1" state="visible" r:id="rId2"/>
@@ -994,8 +994,8 @@
   </sheetPr>
   <dimension ref="A1:J20"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D10" activeCellId="0" sqref="D10"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D6" activeCellId="0" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1156,15 +1156,14 @@
         <v>38</v>
       </c>
       <c r="C5" s="4" t="n">
-        <v>5E-006</v>
+        <v>0</v>
       </c>
       <c r="D5" s="6" t="n">
-        <f aca="false">C5*0.8</f>
-        <v>4E-006</v>
+        <v>0</v>
       </c>
       <c r="E5" s="6" t="n">
         <f aca="false">C5*1.2</f>
-        <v>6E-006</v>
+        <v>0</v>
       </c>
       <c r="F5" s="1" t="n">
         <v>1</v>
@@ -1767,7 +1766,7 @@
   </sheetPr>
   <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
     </sheetView>
   </sheetViews>

</xml_diff>